<commit_message>
MOD 97-10 implementation and unit tests
</commit_message>
<xml_diff>
--- a/Documentation/ISO7064ExamplesWorkbook.xlsx
+++ b/Documentation/ISO7064ExamplesWorkbook.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CheckDigits.Net\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09505FBD-4ADF-41C2-872D-F955E4E992B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4337B4-FAA8-4F39-962E-BB6195694290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{29668144-CB59-4756-8844-303BE2B9F3CC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23520" activeTab="3" xr2:uid="{29668144-CB59-4756-8844-303BE2B9F3CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="MOD 1271-36" sheetId="2" r:id="rId2"/>
     <sheet name="MOD 661-26" sheetId="3" r:id="rId3"/>
+    <sheet name="MOD 97-10" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="68">
   <si>
     <t>A</t>
   </si>
@@ -237,12 +238,18 @@
   <si>
     <t>NS</t>
   </si>
+  <si>
+    <t>ISO/IEC 7064 MOD 97-10</t>
+  </si>
+  <si>
+    <t>"1011339391255432926101144229991433338"</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +261,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF101820"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -279,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -294,11 +308,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -13626,60 +13694,60 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C17">
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C38">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="8" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C59">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="5" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67:C102">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C109:C144">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152:C187">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:F61">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F103">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13692,8 +13760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A402F48E-7D2E-4A97-B8F3-3C3001D1588A}">
   <dimension ref="A1:O165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19216,34 +19284,2781 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C17 C140:C165">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C38">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C59">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C91 C97:C134">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF67E24C-1E84-413B-9210-17598F74D757}">
+  <dimension ref="A1:M103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M93" sqref="M93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1">
+        <v>97</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1">
+        <f>TRUNC(2147483647/B3)</f>
+        <v>214748364</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4">
+        <v>123456</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="4">
+        <v>76</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f>(C12+B13)*$B$3</f>
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <f>MOD((D12+B13)*$B$3,$B$2)</f>
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <f>MOD(D13*$B$3,$B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <f>$B$2+1-F13</f>
+        <v>95</v>
+      </c>
+      <c r="H13">
+        <f>(G13-I13)/$B$3</f>
+        <v>9</v>
+      </c>
+      <c r="I13">
+        <f>MOD(G13,$B$3)</f>
+        <v>5</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:C17" si="0">(C13+B14)*$B$3</f>
+        <v>120</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D17" si="1">MOD((D13+B14)*$B$3,$B$2)</f>
+        <v>23</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F17" si="2">MOD(D14*$B$3,$B$2)</f>
+        <v>36</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G17" si="3">$B$2+1-F14</f>
+        <v>62</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H17" si="4">(G14-I14)/$B$3</f>
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14:I17" si="5">MOD(G14,$B$3)</f>
+        <v>2</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1230</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>12340</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>123450</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18" si="6">(C17+B18)*$B$3</f>
+        <v>1234560</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18" si="7">MOD((D17+B18)*$B$3,$B$2)</f>
+        <v>41</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ref="F18" si="8">MOD(D18*$B$3,$B$2)</f>
+        <v>22</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18" si="9">$B$2+1-F18</f>
+        <v>76</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18" si="10">(G18-I18)/$B$3</f>
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ref="I18" si="11">MOD(G18,$B$3)</f>
+        <v>6</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1632175818351010</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="4">
+        <v>38</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <f>(C25+B26)*$B$3</f>
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <f>MOD((D25+B26)*$B$3,$B$2)</f>
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <f>MOD(D26*$B$3,$B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="G26" s="1">
+        <f>$B$2+1-F26</f>
+        <v>95</v>
+      </c>
+      <c r="H26" s="1">
+        <f>(G26-I26)/$B$3</f>
+        <v>9</v>
+      </c>
+      <c r="I26">
+        <f>MOD(G26,$B$3)</f>
+        <v>5</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27:C39" si="12">(C26+B27)*$B$3</f>
+        <v>160</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ref="D27:D39" si="13">MOD((D26+B27)*$B$3,$B$2)</f>
+        <v>63</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:F39" si="14">MOD(D27*$B$3,$B$2)</f>
+        <v>48</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" ref="G27:G39" si="15">$B$2+1-F27</f>
+        <v>50</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" ref="H27:H39" si="16">(G27-I27)/$B$3</f>
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27:I39" si="17">MOD(G27,$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="12"/>
+        <v>1630</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="13"/>
+        <v>78</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="15"/>
+        <v>94</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="12"/>
+        <v>16320</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="13"/>
+        <v>24</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="14"/>
+        <v>46</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="15"/>
+        <v>52</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>1</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="12"/>
+        <v>163210</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="13"/>
+        <v>56</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="14"/>
+        <v>75</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="15"/>
+        <v>23</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="12"/>
+        <v>1632170</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="13"/>
+        <v>48</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="14"/>
+        <v>92</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="12"/>
+        <v>16321750</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="14"/>
+        <v>62</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="15"/>
+        <v>36</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="12"/>
+        <v>163217580</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="14"/>
+        <v>62</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="15"/>
+        <v>36</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="12"/>
+        <v>1632175810</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="13"/>
+        <v>72</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="14"/>
+        <v>41</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="15"/>
+        <v>57</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="12"/>
+        <v>16321758180</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="13"/>
+        <v>24</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="14"/>
+        <v>46</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="15"/>
+        <v>52</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>3</v>
+      </c>
+      <c r="B36" s="1">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="12"/>
+        <v>163217581830</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="13"/>
+        <v>76</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="14"/>
+        <v>81</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="15"/>
+        <v>17</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="12"/>
+        <v>1632175818350</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="13"/>
+        <v>34</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="14"/>
+        <v>49</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="15"/>
+        <v>49</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="17"/>
+        <v>9</v>
+      </c>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="12"/>
+        <v>16321758183510</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="13"/>
+        <v>59</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="15"/>
+        <v>90</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>9</v>
+      </c>
+      <c r="B39" s="1">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="12"/>
+        <v>163217581835190</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="15"/>
+        <v>88</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="16"/>
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ref="C40:C41" si="18">(C39+B40)*$B$3</f>
+        <v>1632175818351910</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ref="D40:D41" si="19">MOD((D39+B40)*$B$3,$B$2)</f>
+        <v>20</v>
+      </c>
+      <c r="F40">
+        <f t="shared" ref="F40:F41" si="20">MOD(D40*$B$3,$B$2)</f>
+        <v>6</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" ref="G40:G41" si="21">$B$2+1-F40</f>
+        <v>92</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" ref="H40:H41" si="22">(G40-I40)/$B$3</f>
+        <v>9</v>
+      </c>
+      <c r="I40">
+        <f t="shared" ref="I40:I41" si="23">MOD(G40,$B$3)</f>
+        <v>2</v>
+      </c>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="18"/>
+        <v>1.63217581835191E+16</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="20"/>
+        <v>60</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="21"/>
+        <v>38</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="23"/>
+        <v>8</v>
+      </c>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="M42" s="1"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="M43" s="1"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="4">
+        <v>38</v>
+      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="M47" s="1"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>1</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <f>(C48+B49)*$B$3</f>
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <f>MOD((D48+B49)*$B$3,$B$2)</f>
+        <v>10</v>
+      </c>
+      <c r="F49">
+        <f>MOD(D49*$B$3,$B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="G49" s="1">
+        <f>$B$2+1-F49</f>
+        <v>95</v>
+      </c>
+      <c r="H49" s="1">
+        <f>(G49-I49)/$B$3</f>
+        <v>9</v>
+      </c>
+      <c r="I49">
+        <f>MOD(G49,$B$3)</f>
+        <v>5</v>
+      </c>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ref="C50:C68" si="24">(C49+B50)*$B$3</f>
+        <v>100</v>
+      </c>
+      <c r="D50">
+        <f t="shared" ref="D50:D68" si="25">MOD((D49+B50)*$B$3,$B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="F50">
+        <f t="shared" ref="F50:F68" si="26">MOD(D50*$B$3,$B$2)</f>
+        <v>30</v>
+      </c>
+      <c r="G50" s="1">
+        <f t="shared" ref="G50:G68" si="27">$B$2+1-F50</f>
+        <v>68</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" ref="H50:H68" si="28">(G50-I50)/$B$3</f>
+        <v>6</v>
+      </c>
+      <c r="I50">
+        <f t="shared" ref="I50:I68" si="29">MOD(G50,$B$3)</f>
+        <v>8</v>
+      </c>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="M50" s="1"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>1</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="24"/>
+        <v>1010</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="25"/>
+        <v>40</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="26"/>
+        <v>12</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="27"/>
+        <v>86</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="28"/>
+        <v>8</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="29"/>
+        <v>6</v>
+      </c>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="M51" s="1"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>1</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="24"/>
+        <v>10110</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="25"/>
+        <v>22</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="26"/>
+        <v>26</v>
+      </c>
+      <c r="G52" s="1">
+        <f t="shared" si="27"/>
+        <v>72</v>
+      </c>
+      <c r="H52" s="1">
+        <f t="shared" si="28"/>
+        <v>7</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="J52" s="1"/>
+      <c r="M52" s="1"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>3</v>
+      </c>
+      <c r="B53" s="1">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="24"/>
+        <v>101130</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="25"/>
+        <v>56</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="26"/>
+        <v>75</v>
+      </c>
+      <c r="G53" s="1">
+        <f t="shared" si="27"/>
+        <v>23</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="J53" s="1"/>
+      <c r="M53" s="1"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>3</v>
+      </c>
+      <c r="B54" s="1">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="24"/>
+        <v>1011330</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="25"/>
+        <v>8</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="26"/>
+        <v>80</v>
+      </c>
+      <c r="G54" s="1">
+        <f t="shared" si="27"/>
+        <v>18</v>
+      </c>
+      <c r="H54" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="29"/>
+        <v>8</v>
+      </c>
+      <c r="J54" s="1"/>
+      <c r="M54" s="1"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>9</v>
+      </c>
+      <c r="B55" s="1">
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="24"/>
+        <v>10113390</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="25"/>
+        <v>73</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="26"/>
+        <v>51</v>
+      </c>
+      <c r="G55" s="1">
+        <f t="shared" si="27"/>
+        <v>47</v>
+      </c>
+      <c r="H55" s="1">
+        <f t="shared" si="28"/>
+        <v>4</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="J55" s="1"/>
+      <c r="M55" s="1"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>3</v>
+      </c>
+      <c r="B56" s="1">
+        <v>3</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="24"/>
+        <v>101133930</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="25"/>
+        <v>81</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="26"/>
+        <v>34</v>
+      </c>
+      <c r="G56" s="1">
+        <f t="shared" si="27"/>
+        <v>64</v>
+      </c>
+      <c r="H56" s="1">
+        <f t="shared" si="28"/>
+        <v>6</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="J56" s="1"/>
+      <c r="M56" s="1"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>9</v>
+      </c>
+      <c r="B57" s="1">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="24"/>
+        <v>1011339390</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="25"/>
+        <v>27</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="26"/>
+        <v>76</v>
+      </c>
+      <c r="G57" s="1">
+        <f t="shared" si="27"/>
+        <v>22</v>
+      </c>
+      <c r="H57" s="1">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="J57" s="2"/>
+      <c r="K57" s="3"/>
+      <c r="M57" s="1"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>1</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="24"/>
+        <v>10113393910</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="25"/>
+        <v>86</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="26"/>
+        <v>84</v>
+      </c>
+      <c r="G58" s="1">
+        <f t="shared" si="27"/>
+        <v>14</v>
+      </c>
+      <c r="H58" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="J58" s="1"/>
+      <c r="M58" s="1"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>2</v>
+      </c>
+      <c r="B59" s="1">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="24"/>
+        <v>101133939120</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="25"/>
+        <v>7</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="26"/>
+        <v>70</v>
+      </c>
+      <c r="G59" s="1">
+        <f t="shared" si="27"/>
+        <v>28</v>
+      </c>
+      <c r="H59" s="1">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="29"/>
+        <v>8</v>
+      </c>
+      <c r="J59" s="1"/>
+      <c r="M59" s="1"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>5</v>
+      </c>
+      <c r="B60" s="1">
+        <v>5</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="24"/>
+        <v>1011339391250</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="25"/>
+        <v>23</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="26"/>
+        <v>36</v>
+      </c>
+      <c r="G60" s="1">
+        <f t="shared" si="27"/>
+        <v>62</v>
+      </c>
+      <c r="H60" s="1">
+        <f t="shared" si="28"/>
+        <v>6</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="J60" s="1"/>
+      <c r="M60" s="1"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>5</v>
+      </c>
+      <c r="B61" s="1">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="24"/>
+        <v>10113393912550</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="25"/>
+        <v>86</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="26"/>
+        <v>84</v>
+      </c>
+      <c r="G61" s="1">
+        <f t="shared" si="27"/>
+        <v>14</v>
+      </c>
+      <c r="H61" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="J61" s="1"/>
+      <c r="M61" s="1"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>4</v>
+      </c>
+      <c r="B62" s="1">
+        <v>4</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="24"/>
+        <v>101133939125540</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="25"/>
+        <v>27</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="26"/>
+        <v>76</v>
+      </c>
+      <c r="G62" s="1">
+        <f t="shared" si="27"/>
+        <v>22</v>
+      </c>
+      <c r="H62" s="1">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="J62" s="1"/>
+      <c r="M62" s="1"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>3</v>
+      </c>
+      <c r="B63" s="1">
+        <v>3</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="24"/>
+        <v>1011339391255430</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="25"/>
+        <v>9</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="26"/>
+        <v>90</v>
+      </c>
+      <c r="G63" s="1">
+        <f t="shared" si="27"/>
+        <v>8</v>
+      </c>
+      <c r="H63" s="1">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="29"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>2</v>
+      </c>
+      <c r="B64" s="1">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="24"/>
+        <v>1.011339391255432E+16</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="25"/>
+        <v>13</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="26"/>
+        <v>33</v>
+      </c>
+      <c r="G64" s="1">
+        <f t="shared" si="27"/>
+        <v>65</v>
+      </c>
+      <c r="H64" s="1">
+        <f t="shared" si="28"/>
+        <v>6</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="29"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>9</v>
+      </c>
+      <c r="B65" s="1">
+        <v>9</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="24"/>
+        <v>1.0113393912554328E+17</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="25"/>
+        <v>26</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="26"/>
+        <v>66</v>
+      </c>
+      <c r="G65" s="1">
+        <f t="shared" si="27"/>
+        <v>32</v>
+      </c>
+      <c r="H65" s="1">
+        <f t="shared" si="28"/>
+        <v>3</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>2</v>
+      </c>
+      <c r="B66" s="1">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="24"/>
+        <v>1.0113393912554328E+18</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="25"/>
+        <v>86</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="26"/>
+        <v>84</v>
+      </c>
+      <c r="G66" s="1">
+        <f t="shared" si="27"/>
+        <v>14</v>
+      </c>
+      <c r="H66" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>6</v>
+      </c>
+      <c r="B67" s="1">
+        <v>6</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="24"/>
+        <v>1.0113393912554328E+19</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="25"/>
+        <v>47</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="26"/>
+        <v>82</v>
+      </c>
+      <c r="G67" s="1">
+        <f t="shared" si="27"/>
+        <v>16</v>
+      </c>
+      <c r="H67" s="1">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="29"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>1</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="24"/>
+        <v>1.0113393912554327E+20</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="25"/>
+        <v>92</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="26"/>
+        <v>47</v>
+      </c>
+      <c r="G68" s="1">
+        <f t="shared" si="27"/>
+        <v>51</v>
+      </c>
+      <c r="H68" s="1">
+        <f t="shared" si="28"/>
+        <v>5</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <f t="shared" ref="C69:C83" si="30">(C68+B69)*$B$3</f>
+        <v>1.0113393912554327E+21</v>
+      </c>
+      <c r="D69">
+        <f t="shared" ref="D69:D83" si="31">MOD((D68+B69)*$B$3,$B$2)</f>
+        <v>47</v>
+      </c>
+      <c r="F69">
+        <f t="shared" ref="F69:F83" si="32">MOD(D69*$B$3,$B$2)</f>
+        <v>82</v>
+      </c>
+      <c r="G69" s="1">
+        <f t="shared" ref="G69:G83" si="33">$B$2+1-F69</f>
+        <v>16</v>
+      </c>
+      <c r="H69" s="1">
+        <f t="shared" ref="H69:H83" si="34">(G69-I69)/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <f t="shared" ref="I69:I83" si="35">MOD(G69,$B$3)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>1</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554327E+22</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="31"/>
+        <v>92</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="32"/>
+        <v>47</v>
+      </c>
+      <c r="G70" s="1">
+        <f t="shared" si="33"/>
+        <v>51</v>
+      </c>
+      <c r="H70" s="1">
+        <f t="shared" si="34"/>
+        <v>5</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>1</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554327E+23</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="31"/>
+        <v>57</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="32"/>
+        <v>85</v>
+      </c>
+      <c r="G71" s="1">
+        <f t="shared" si="33"/>
+        <v>13</v>
+      </c>
+      <c r="H71" s="1">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="35"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>4</v>
+      </c>
+      <c r="B72" s="1">
+        <v>4</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554326E+24</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="31"/>
+        <v>28</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="32"/>
+        <v>86</v>
+      </c>
+      <c r="G72" s="1">
+        <f t="shared" si="33"/>
+        <v>12</v>
+      </c>
+      <c r="H72" s="1">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="35"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>4</v>
+      </c>
+      <c r="B73" s="1">
+        <v>4</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554325E+25</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="31"/>
+        <v>29</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="32"/>
+        <v>96</v>
+      </c>
+      <c r="G73" s="1">
+        <f t="shared" si="33"/>
+        <v>2</v>
+      </c>
+      <c r="H73" s="1">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="35"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>2</v>
+      </c>
+      <c r="B74" s="1">
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554325E+26</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="31"/>
+        <v>19</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="32"/>
+        <v>93</v>
+      </c>
+      <c r="G74" s="1">
+        <f t="shared" si="33"/>
+        <v>5</v>
+      </c>
+      <c r="H74" s="1">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="35"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>2</v>
+      </c>
+      <c r="B75" s="1">
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554325E+27</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="31"/>
+        <v>16</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="32"/>
+        <v>63</v>
+      </c>
+      <c r="G75" s="1">
+        <f t="shared" si="33"/>
+        <v>35</v>
+      </c>
+      <c r="H75" s="1">
+        <f t="shared" si="34"/>
+        <v>3</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="35"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>9</v>
+      </c>
+      <c r="B76" s="1">
+        <v>9</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554325E+28</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="31"/>
+        <v>56</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="32"/>
+        <v>75</v>
+      </c>
+      <c r="G76" s="1">
+        <f t="shared" si="33"/>
+        <v>23</v>
+      </c>
+      <c r="H76" s="1">
+        <f t="shared" si="34"/>
+        <v>2</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="35"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>9</v>
+      </c>
+      <c r="B77" s="1">
+        <v>9</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554325E+29</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="31"/>
+        <v>68</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="G77" s="1">
+        <f t="shared" si="33"/>
+        <v>97</v>
+      </c>
+      <c r="H77" s="1">
+        <f t="shared" si="34"/>
+        <v>9</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="35"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>9</v>
+      </c>
+      <c r="B78" s="1">
+        <v>9</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554326E+30</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="31"/>
+        <v>91</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="32"/>
+        <v>37</v>
+      </c>
+      <c r="G78" s="1">
+        <f t="shared" si="33"/>
+        <v>61</v>
+      </c>
+      <c r="H78" s="1">
+        <f t="shared" si="34"/>
+        <v>6</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>1</v>
+      </c>
+      <c r="B79" s="1">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554326E+31</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="31"/>
+        <v>47</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="32"/>
+        <v>82</v>
+      </c>
+      <c r="G79" s="1">
+        <f t="shared" si="33"/>
+        <v>16</v>
+      </c>
+      <c r="H79" s="1">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="35"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>4</v>
+      </c>
+      <c r="B80" s="1">
+        <v>4</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554326E+32</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="31"/>
+        <v>25</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="32"/>
+        <v>56</v>
+      </c>
+      <c r="G80" s="1">
+        <f t="shared" si="33"/>
+        <v>42</v>
+      </c>
+      <c r="H80" s="1">
+        <f t="shared" si="34"/>
+        <v>4</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="35"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>3</v>
+      </c>
+      <c r="B81" s="1">
+        <v>3</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554327E+33</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="31"/>
+        <v>86</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="32"/>
+        <v>84</v>
+      </c>
+      <c r="G81" s="1">
+        <f t="shared" si="33"/>
+        <v>14</v>
+      </c>
+      <c r="H81" s="1">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="35"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>3</v>
+      </c>
+      <c r="B82" s="1">
+        <v>3</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554326E+34</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="31"/>
+        <v>17</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="32"/>
+        <v>73</v>
+      </c>
+      <c r="G82" s="1">
+        <f t="shared" si="33"/>
+        <v>25</v>
+      </c>
+      <c r="H82" s="1">
+        <f t="shared" si="34"/>
+        <v>2</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="35"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>3</v>
+      </c>
+      <c r="B83" s="1">
+        <v>3</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="30"/>
+        <v>1.0113393912554326E+35</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="31"/>
+        <v>6</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="32"/>
+        <v>60</v>
+      </c>
+      <c r="G83" s="1">
+        <f t="shared" si="33"/>
+        <v>38</v>
+      </c>
+      <c r="H83" s="1">
+        <f t="shared" si="34"/>
+        <v>3</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="35"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>0</v>
+      </c>
+      <c r="B94" s="1">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <f t="shared" ref="C94:C103" si="36">B94*$B$3</f>
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <f t="shared" ref="D94:D103" si="37">MOD(B94*$B$3,$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <f t="shared" ref="F94:F103" si="38">MOD(D94*$B$3,$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="G94" s="1">
+        <f t="shared" ref="G94:G103" si="39">$B$2+1-F94</f>
+        <v>98</v>
+      </c>
+      <c r="H94" s="1">
+        <f t="shared" ref="H94:H103" si="40">(G94-I94)/$B$3</f>
+        <v>9</v>
+      </c>
+      <c r="I94">
+        <f t="shared" ref="I94:I103" si="41">MOD(G94,$B$3)</f>
+        <v>8</v>
+      </c>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>1</v>
+      </c>
+      <c r="B95" s="1">
+        <v>1</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="36"/>
+        <v>10</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="37"/>
+        <v>10</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="38"/>
+        <v>3</v>
+      </c>
+      <c r="G95" s="1">
+        <f t="shared" si="39"/>
+        <v>95</v>
+      </c>
+      <c r="H95" s="1">
+        <f t="shared" si="40"/>
+        <v>9</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="41"/>
+        <v>5</v>
+      </c>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>2</v>
+      </c>
+      <c r="B96" s="1">
+        <v>2</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="36"/>
+        <v>20</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="37"/>
+        <v>20</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="38"/>
+        <v>6</v>
+      </c>
+      <c r="G96" s="1">
+        <f t="shared" si="39"/>
+        <v>92</v>
+      </c>
+      <c r="H96" s="1">
+        <f t="shared" si="40"/>
+        <v>9</v>
+      </c>
+      <c r="I96">
+        <f t="shared" si="41"/>
+        <v>2</v>
+      </c>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>3</v>
+      </c>
+      <c r="B97" s="1">
+        <v>3</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="36"/>
+        <v>30</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="37"/>
+        <v>30</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="38"/>
+        <v>9</v>
+      </c>
+      <c r="G97" s="1">
+        <f t="shared" si="39"/>
+        <v>89</v>
+      </c>
+      <c r="H97" s="1">
+        <f t="shared" si="40"/>
+        <v>8</v>
+      </c>
+      <c r="I97">
+        <f t="shared" si="41"/>
+        <v>9</v>
+      </c>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>4</v>
+      </c>
+      <c r="B98" s="1">
+        <v>4</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="36"/>
+        <v>40</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="37"/>
+        <v>40</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="38"/>
+        <v>12</v>
+      </c>
+      <c r="G98" s="1">
+        <f t="shared" si="39"/>
+        <v>86</v>
+      </c>
+      <c r="H98" s="1">
+        <f t="shared" si="40"/>
+        <v>8</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="41"/>
+        <v>6</v>
+      </c>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>5</v>
+      </c>
+      <c r="B99" s="1">
+        <v>5</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="36"/>
+        <v>50</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="37"/>
+        <v>50</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="38"/>
+        <v>15</v>
+      </c>
+      <c r="G99" s="1">
+        <f t="shared" si="39"/>
+        <v>83</v>
+      </c>
+      <c r="H99" s="1">
+        <f t="shared" si="40"/>
+        <v>8</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="41"/>
+        <v>3</v>
+      </c>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>6</v>
+      </c>
+      <c r="B100" s="1">
+        <v>6</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="36"/>
+        <v>60</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="37"/>
+        <v>60</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="38"/>
+        <v>18</v>
+      </c>
+      <c r="G100" s="1">
+        <f t="shared" si="39"/>
+        <v>80</v>
+      </c>
+      <c r="H100" s="1">
+        <f t="shared" si="40"/>
+        <v>8</v>
+      </c>
+      <c r="I100">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>7</v>
+      </c>
+      <c r="B101" s="1">
+        <v>7</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="36"/>
+        <v>70</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="37"/>
+        <v>70</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="38"/>
+        <v>21</v>
+      </c>
+      <c r="G101" s="1">
+        <f t="shared" si="39"/>
+        <v>77</v>
+      </c>
+      <c r="H101" s="1">
+        <f t="shared" si="40"/>
+        <v>7</v>
+      </c>
+      <c r="I101">
+        <f t="shared" si="41"/>
+        <v>7</v>
+      </c>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>8</v>
+      </c>
+      <c r="B102" s="1">
+        <v>8</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="36"/>
+        <v>80</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="37"/>
+        <v>80</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="38"/>
+        <v>24</v>
+      </c>
+      <c r="G102" s="1">
+        <f t="shared" si="39"/>
+        <v>74</v>
+      </c>
+      <c r="H102" s="1">
+        <f t="shared" si="40"/>
+        <v>7</v>
+      </c>
+      <c r="I102">
+        <f t="shared" si="41"/>
+        <v>4</v>
+      </c>
+      <c r="J102" s="1"/>
+      <c r="K102" s="1"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>9</v>
+      </c>
+      <c r="B103" s="1">
+        <v>9</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="36"/>
+        <v>90</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="37"/>
+        <v>90</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="38"/>
+        <v>27</v>
+      </c>
+      <c r="G103" s="1">
+        <f t="shared" si="39"/>
+        <v>71</v>
+      </c>
+      <c r="H103" s="1">
+        <f t="shared" si="40"/>
+        <v>7</v>
+      </c>
+      <c r="I103">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="J103" s="1"/>
+      <c r="K103" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C94:C103 C13:C18">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
+      <formula>$B$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:C41 C87:C88">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+      <formula>$B$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C86">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>$B$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MOD 27,26 implementation and unit tests
</commit_message>
<xml_diff>
--- a/Documentation/ISO7064ExamplesWorkbook.xlsx
+++ b/Documentation/ISO7064ExamplesWorkbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CheckDigits.Net\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A328F1E-3E38-436A-B846-20CE1B1A24D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C392AD34-E64E-443A-AE30-EBBB31A49FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{29668144-CB59-4756-8844-303BE2B9F3CC}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="5" xr2:uid="{29668144-CB59-4756-8844-303BE2B9F3CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="MOD 661-26" sheetId="3" r:id="rId3"/>
     <sheet name="MOD 97-10" sheetId="4" r:id="rId4"/>
     <sheet name="MOD 11,10" sheetId="5" r:id="rId5"/>
+    <sheet name="MOD 27,26" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="81">
   <si>
     <t>A</t>
   </si>
@@ -269,6 +270,21 @@
   <si>
     <t>"12345678901234567890123456"</t>
   </si>
+  <si>
+    <t>ISO/IEC 7064 MOD 27,26</t>
+  </si>
+  <si>
+    <t>AEIOU</t>
+  </si>
+  <si>
+    <t>Check Character</t>
+  </si>
+  <si>
+    <t>QWERTYDVORAK</t>
+  </si>
+  <si>
+    <t>THISISATESTTHISISONLYATEST</t>
+  </si>
 </sst>
 </file>
 
@@ -347,7 +363,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -13785,60 +13831,60 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C17">
-    <cfRule type="cellIs" dxfId="31" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="13" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C38">
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="8" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C59">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67:C102">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C109:C144">
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152:C187">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:F61">
-    <cfRule type="cellIs" dxfId="21" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="12" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="16" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F103">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="11" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13852,7 +13898,7 @@
   <dimension ref="A1:O165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="N12" sqref="N12:O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19375,31 +19421,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C17 C140:C165">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C38">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C59">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C91 C97:C134">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22129,23 +22175,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C18 C94:C103">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C41">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C88">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22158,8 +22204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5584CF-414C-4EBC-8048-68A52149ECD3}">
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24538,31 +24584,1868 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C12:C16">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:C31 C40:C47">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C71">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80:C105">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C113:C122">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947D9567-54F5-4216-AEA8-9692E2EF65CA}">
+  <dimension ref="A1:M70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="1">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="F10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1">
+        <f>LOOKUP(A12,$L$11:$L$36,$M$11:$M$36)</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f>F11+B12</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>IF(MOD(C12,$B$2)=0,$B$2,MOD(C12,$B$2))</f>
+        <v>26</v>
+      </c>
+      <c r="E12">
+        <f>D12*2</f>
+        <v>52</v>
+      </c>
+      <c r="F12">
+        <f>MOD(E12,$B$3)</f>
+        <v>25</v>
+      </c>
+      <c r="H12">
+        <f>MOD(($B$2-F12+1),$B$3)</f>
+        <v>2</v>
+      </c>
+      <c r="I12" t="str">
+        <f>LOOKUP(H12,$M$11:$M$36,$L$11:$L$36)</f>
+        <v>C</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" ref="B13:B15" si="0">LOOKUP(A13,$L$11:$L$36,$M$11:$M$36)</f>
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:C15" si="1">F12+B13</f>
+        <v>29</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:D15" si="2">IF(MOD(C13,$B$2)=0,$B$2,MOD(C13,$B$2))</f>
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:E15" si="3">D13*2</f>
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:F15" si="4">MOD(E13,$B$3)</f>
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13:H15" si="5">MOD(($B$2-F13+1),$B$3)</f>
+        <v>21</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" ref="I13:I16" si="6">LOOKUP(H13,$M$11:$M$36,$L$11:$L$36)</f>
+        <v>V</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="6"/>
+        <v>Z</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="6"/>
+        <v>Y</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1">
+        <f>LOOKUP(A16,$L$11:$L$36,$M$11:$M$36)</f>
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <f>F15+B16</f>
+        <v>23</v>
+      </c>
+      <c r="D16">
+        <f>IF(MOD(C16,$B$2)=0,$B$2,MOD(C16,$B$2))</f>
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <f>D16*2</f>
+        <v>46</v>
+      </c>
+      <c r="F16">
+        <f>MOD(E16,$B$3)</f>
+        <v>19</v>
+      </c>
+      <c r="H16">
+        <f>MOD(($B$2-F16+1),$B$3)</f>
+        <v>8</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="6"/>
+        <v>I</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M16" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M19" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="L22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="F23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M23" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M24" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1">
+        <f>LOOKUP(A25,$L$11:$L$36,$M$11:$M$36)</f>
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <f>F24+B25</f>
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <f>IF(MOD(C25,$B$2)=0,$B$2,MOD(C25,$B$2))</f>
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <f>D25*2</f>
+        <v>32</v>
+      </c>
+      <c r="F25">
+        <f>MOD(E25,$B$3)</f>
+        <v>5</v>
+      </c>
+      <c r="H25">
+        <f>MOD(($B$2-F25+1),$B$3)</f>
+        <v>22</v>
+      </c>
+      <c r="I25" t="str">
+        <f>LOOKUP(H25,$M$11:$M$36,$L$11:$L$36)</f>
+        <v>W</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M25" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" ref="B26:B36" si="7">LOOKUP(A26,$L$11:$L$36,$M$11:$M$36)</f>
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:C36" si="8">F25+B26</f>
+        <v>27</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ref="D26:D36" si="9">IF(MOD(C26,$B$2)=0,$B$2,MOD(C26,$B$2))</f>
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26:E36" si="10">D26*2</f>
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ref="F26:F36" si="11">MOD(E26,$B$3)</f>
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <f t="shared" ref="H26:H36" si="12">MOD(($B$2-F26+1),$B$3)</f>
+        <v>25</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" ref="I26:I36" si="13">LOOKUP(H26,$M$11:$M$36,$L$11:$L$36)</f>
+        <v>Z</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M26" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="13"/>
+        <v>P</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="12"/>
+        <v>21</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="13"/>
+        <v>V</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="7"/>
+        <v>19</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="10"/>
+        <v>50</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="11"/>
+        <v>23</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="13"/>
+        <v>E</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M29" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="7"/>
+        <v>24</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="8"/>
+        <v>47</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="9"/>
+        <v>21</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="10"/>
+        <v>42</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="11"/>
+        <v>15</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="12"/>
+        <v>12</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="13"/>
+        <v>M</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="9"/>
+        <v>18</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="10"/>
+        <v>36</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="13"/>
+        <v>S</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="7"/>
+        <v>21</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="12"/>
+        <v>19</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="13"/>
+        <v>T</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="10"/>
+        <v>44</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="11"/>
+        <v>17</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="13"/>
+        <v>K</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M33" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="8"/>
+        <v>34</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="11"/>
+        <v>16</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="12"/>
+        <v>11</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="13"/>
+        <v>L</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M34" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="10"/>
+        <v>32</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="12"/>
+        <v>22</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="13"/>
+        <v>W</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M35" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="10"/>
+        <v>30</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="12"/>
+        <v>24</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="13"/>
+        <v>Y</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="F43" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="1">
+        <f>LOOKUP(A45,$L$11:$L$36,$M$11:$M$36)</f>
+        <v>19</v>
+      </c>
+      <c r="C45">
+        <f>F44+B45</f>
+        <v>19</v>
+      </c>
+      <c r="D45">
+        <f>IF(MOD(C45,$B$2)=0,$B$2,MOD(C45,$B$2))</f>
+        <v>19</v>
+      </c>
+      <c r="E45">
+        <f>D45*2</f>
+        <v>38</v>
+      </c>
+      <c r="F45">
+        <f>MOD(E45,$B$3)</f>
+        <v>11</v>
+      </c>
+      <c r="H45">
+        <f>MOD(($B$2-F45+1),$B$3)</f>
+        <v>16</v>
+      </c>
+      <c r="I45" t="str">
+        <f>LOOKUP(H45,$M$11:$M$36,$L$11:$L$36)</f>
+        <v>Q</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" ref="B46:B70" si="14">LOOKUP(A46,$L$11:$L$36,$M$11:$M$36)</f>
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ref="C46:C70" si="15">F45+B46</f>
+        <v>18</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ref="D46:D70" si="16">IF(MOD(C46,$B$2)=0,$B$2,MOD(C46,$B$2))</f>
+        <v>18</v>
+      </c>
+      <c r="E46">
+        <f t="shared" ref="E46:E70" si="17">D46*2</f>
+        <v>36</v>
+      </c>
+      <c r="F46">
+        <f t="shared" ref="F46:F70" si="18">MOD(E46,$B$3)</f>
+        <v>9</v>
+      </c>
+      <c r="H46">
+        <f t="shared" ref="H46:H70" si="19">MOD(($B$2-F46+1),$B$3)</f>
+        <v>18</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" ref="I46:I70" si="20">LOOKUP(H46,$M$11:$M$36,$L$11:$L$36)</f>
+        <v>S</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="15"/>
+        <v>17</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="16"/>
+        <v>17</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="17"/>
+        <v>34</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="18"/>
+        <v>7</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="19"/>
+        <v>20</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="20"/>
+        <v>U</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" si="14"/>
+        <v>18</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="16"/>
+        <v>25</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="17"/>
+        <v>50</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="18"/>
+        <v>23</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="19"/>
+        <v>4</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="20"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="15"/>
+        <v>31</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="19"/>
+        <v>17</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="20"/>
+        <v>R</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" si="14"/>
+        <v>18</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="15"/>
+        <v>28</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="19"/>
+        <v>23</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="20"/>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="15"/>
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="19"/>
+        <v>19</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="20"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="1">
+        <f t="shared" si="14"/>
+        <v>19</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="15"/>
+        <v>27</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="20"/>
+        <v>Z</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="1">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="18"/>
+        <v>12</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="19"/>
+        <v>15</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="20"/>
+        <v>P</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="1">
+        <f t="shared" si="14"/>
+        <v>18</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="19"/>
+        <v>19</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="20"/>
+        <v>T</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="1">
+        <f t="shared" si="14"/>
+        <v>19</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="15"/>
+        <v>27</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="19"/>
+        <v>25</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="20"/>
+        <v>Z</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" s="1">
+        <f t="shared" si="14"/>
+        <v>19</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="15"/>
+        <v>21</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="16"/>
+        <v>21</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="17"/>
+        <v>42</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="18"/>
+        <v>15</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="19"/>
+        <v>12</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="20"/>
+        <v>M</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="1">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="15"/>
+        <v>22</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="16"/>
+        <v>22</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="17"/>
+        <v>44</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="18"/>
+        <v>17</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="19"/>
+        <v>10</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="20"/>
+        <v>K</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="1">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="15"/>
+        <v>25</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="16"/>
+        <v>25</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="17"/>
+        <v>50</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="18"/>
+        <v>23</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="19"/>
+        <v>4</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="20"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="1">
+        <f t="shared" si="14"/>
+        <v>18</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="15"/>
+        <v>41</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="19"/>
+        <v>24</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="20"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" s="1">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="15"/>
+        <v>11</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="16"/>
+        <v>11</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="17"/>
+        <v>22</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="18"/>
+        <v>22</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="19"/>
+        <v>5</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="20"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" s="1">
+        <f t="shared" si="14"/>
+        <v>18</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="15"/>
+        <v>40</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="16"/>
+        <v>14</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="17"/>
+        <v>28</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="19"/>
+        <v>26</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="20"/>
+        <v>Z</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" s="1">
+        <f t="shared" si="14"/>
+        <v>14</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="15"/>
+        <v>15</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="17"/>
+        <v>30</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="19"/>
+        <v>24</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="20"/>
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" s="1">
+        <f t="shared" si="14"/>
+        <v>13</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="15"/>
+        <v>16</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="16"/>
+        <v>16</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="17"/>
+        <v>32</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="19"/>
+        <v>22</v>
+      </c>
+      <c r="I63" t="str">
+        <f t="shared" si="20"/>
+        <v>W</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" s="1">
+        <f t="shared" si="14"/>
+        <v>11</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="15"/>
+        <v>16</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="16"/>
+        <v>16</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="17"/>
+        <v>32</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="18"/>
+        <v>5</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="19"/>
+        <v>22</v>
+      </c>
+      <c r="I64" t="str">
+        <f t="shared" si="20"/>
+        <v>W</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B65" s="1">
+        <f t="shared" si="14"/>
+        <v>24</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="15"/>
+        <v>29</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="19"/>
+        <v>21</v>
+      </c>
+      <c r="I65" t="str">
+        <f t="shared" si="20"/>
+        <v>V</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="16"/>
+        <v>6</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="18"/>
+        <v>12</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="19"/>
+        <v>15</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="20"/>
+        <v>P</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="1">
+        <f t="shared" si="14"/>
+        <v>19</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="15"/>
+        <v>31</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="17"/>
+        <v>10</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="19"/>
+        <v>17</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" si="20"/>
+        <v>R</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="1">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="15"/>
+        <v>14</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="16"/>
+        <v>14</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="17"/>
+        <v>28</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="19"/>
+        <v>26</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="20"/>
+        <v>Z</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" s="1">
+        <f t="shared" si="14"/>
+        <v>18</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="15"/>
+        <v>19</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="16"/>
+        <v>19</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="17"/>
+        <v>38</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="18"/>
+        <v>11</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="19"/>
+        <v>16</v>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="20"/>
+        <v>Q</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="1">
+        <f t="shared" si="14"/>
+        <v>19</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="15"/>
+        <v>30</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="19"/>
+        <v>19</v>
+      </c>
+      <c r="I70" t="str">
+        <f t="shared" si="20"/>
+        <v>T</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C12:C16">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C113:C122">
+  <conditionalFormatting sqref="C25:C36">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
+  <conditionalFormatting sqref="C45:C70">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>

</xml_diff>

<commit_message>
Readme updates and cleanup for custom alphabets
</commit_message>
<xml_diff>
--- a/Documentation/ISO7064ExamplesWorkbook.xlsx
+++ b/Documentation/ISO7064ExamplesWorkbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CheckDigits.Net\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE49789-480E-4E86-8563-28464959DE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A947603-616F-4C3D-9580-BB40B1F7A621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="6" xr2:uid="{29668144-CB59-4756-8844-303BE2B9F3CC}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="7" xr2:uid="{29668144-CB59-4756-8844-303BE2B9F3CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="MOD 11,10" sheetId="5" r:id="rId5"/>
     <sheet name="MOD 27,26" sheetId="6" r:id="rId6"/>
     <sheet name="MOD 37,36" sheetId="7" r:id="rId7"/>
+    <sheet name="Danish MOD 29-2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="89">
   <si>
     <t>A</t>
   </si>
@@ -295,6 +296,21 @@
   <si>
     <t>1234567890ABCDEFGHIJKLMNOPQRSTUVWXYZ</t>
   </si>
+  <si>
+    <t>[Danish] MOD 29-2</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>A Umlaut</t>
+  </si>
+  <si>
+    <t>OSlash</t>
+  </si>
 </sst>
 </file>
 
@@ -373,7 +389,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="44">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1116,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89D0F3D-CC63-4CE8-A289-1E368BD8F169}">
   <dimension ref="A2:Y120"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85:B110"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7045,8 +7071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D67299-40B5-46D7-8C2D-E7BD98472505}">
   <dimension ref="A1:P187"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12:O48"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13921,60 +13947,60 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C17">
-    <cfRule type="cellIs" dxfId="42" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="13" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C38">
-    <cfRule type="cellIs" dxfId="41" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="8" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C59">
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67:C102">
-    <cfRule type="cellIs" dxfId="37" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="4" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C109:C144">
-    <cfRule type="cellIs" dxfId="35" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="9" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152:C187">
-    <cfRule type="cellIs" dxfId="34" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:F61">
-    <cfRule type="cellIs" dxfId="32" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="12" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="16" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F103">
-    <cfRule type="cellIs" dxfId="30" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="11" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="15" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13987,8 +14013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A402F48E-7D2E-4A97-B8F3-3C3001D1588A}">
   <dimension ref="A1:O165"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19511,31 +19537,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C17 C140:C165">
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="8" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C38">
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C59">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C91 C97:C134">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22265,23 +22291,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C18 C94:C103">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C41">
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C88">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24674,32 +24700,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C12:C16">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:C31 C40:C47">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:C71">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80:C105">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C113:C122">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29168,32 +29194,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C12:C16">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C36">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C62">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:C96">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C105:C135">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C142:C167">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29205,7 +29231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D6287D-4D2F-4608-A67B-E4FAB43D7DD5}">
   <dimension ref="A1:N186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+    <sheetView topLeftCell="A135" workbookViewId="0">
       <selection activeCell="I151" sqref="I151:I186"/>
     </sheetView>
   </sheetViews>
@@ -33128,31 +33154,31 @@
         <v>0</v>
       </c>
       <c r="B151" s="1">
-        <f>LOOKUP(A151,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" ref="B151:B161" si="35">LOOKUP(A151,$M$4:$M$39,$N$4:$N$39)</f>
         <v>0</v>
       </c>
       <c r="C151">
-        <f>$F$150+B151</f>
+        <f t="shared" ref="C151:C161" si="36">$F$150+B151</f>
         <v>36</v>
       </c>
       <c r="D151">
-        <f>IF(MOD(C151,$B$2)=0,$B$2,MOD(C151,$B$2))</f>
+        <f t="shared" ref="D151:D161" si="37">IF(MOD(C151,$B$2)=0,$B$2,MOD(C151,$B$2))</f>
         <v>36</v>
       </c>
       <c r="E151">
-        <f>D151*2</f>
+        <f t="shared" ref="E151:E161" si="38">D151*2</f>
         <v>72</v>
       </c>
       <c r="F151">
-        <f>MOD(E151,$B$3)</f>
+        <f t="shared" ref="F151:F161" si="39">MOD(E151,$B$3)</f>
         <v>35</v>
       </c>
       <c r="H151">
-        <f t="shared" ref="H151:H160" si="35">MOD(($B$2-F151+1),$B$3)</f>
+        <f t="shared" ref="H151:H160" si="40">MOD(($B$2-F151+1),$B$3)</f>
         <v>2</v>
       </c>
       <c r="I151" s="1">
-        <f>LOOKUP(H151,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" ref="I151:I161" si="41">LOOKUP(H151,$N$4:$N$39,$M$4:$M$39)</f>
         <v>2</v>
       </c>
     </row>
@@ -33161,31 +33187,31 @@
         <v>1</v>
       </c>
       <c r="B152" s="1">
-        <f>LOOKUP(A152,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="C152">
-        <f>$F$150+B152</f>
+        <f t="shared" si="36"/>
         <v>37</v>
       </c>
       <c r="D152">
-        <f>IF(MOD(C152,$B$2)=0,$B$2,MOD(C152,$B$2))</f>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="E152">
-        <f>D152*2</f>
+        <f t="shared" si="38"/>
         <v>2</v>
       </c>
       <c r="F152">
-        <f>MOD(E152,$B$3)</f>
+        <f t="shared" si="39"/>
         <v>2</v>
       </c>
       <c r="H152">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>35</v>
       </c>
       <c r="I152" s="1" t="str">
-        <f>LOOKUP(H152,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" si="41"/>
         <v>Z</v>
       </c>
     </row>
@@ -33194,31 +33220,31 @@
         <v>2</v>
       </c>
       <c r="B153" s="1">
-        <f>LOOKUP(A153,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" si="35"/>
         <v>2</v>
       </c>
       <c r="C153">
-        <f>$F$150+B153</f>
+        <f t="shared" si="36"/>
         <v>38</v>
       </c>
       <c r="D153">
-        <f>IF(MOD(C153,$B$2)=0,$B$2,MOD(C153,$B$2))</f>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="E153">
-        <f>D153*2</f>
+        <f t="shared" si="38"/>
         <v>4</v>
       </c>
       <c r="F153">
-        <f>MOD(E153,$B$3)</f>
+        <f t="shared" si="39"/>
         <v>4</v>
       </c>
       <c r="H153">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>33</v>
       </c>
       <c r="I153" s="1" t="str">
-        <f>LOOKUP(H153,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" si="41"/>
         <v>X</v>
       </c>
     </row>
@@ -33227,31 +33253,31 @@
         <v>3</v>
       </c>
       <c r="B154" s="1">
-        <f>LOOKUP(A154,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" si="35"/>
         <v>3</v>
       </c>
       <c r="C154">
-        <f>$F$150+B154</f>
+        <f t="shared" si="36"/>
         <v>39</v>
       </c>
       <c r="D154">
-        <f>IF(MOD(C154,$B$2)=0,$B$2,MOD(C154,$B$2))</f>
+        <f t="shared" si="37"/>
         <v>3</v>
       </c>
       <c r="E154">
-        <f>D154*2</f>
+        <f t="shared" si="38"/>
         <v>6</v>
       </c>
       <c r="F154">
-        <f>MOD(E154,$B$3)</f>
+        <f t="shared" si="39"/>
         <v>6</v>
       </c>
       <c r="H154">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>31</v>
       </c>
       <c r="I154" s="1" t="str">
-        <f>LOOKUP(H154,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" si="41"/>
         <v>V</v>
       </c>
     </row>
@@ -33260,31 +33286,31 @@
         <v>4</v>
       </c>
       <c r="B155" s="1">
-        <f>LOOKUP(A155,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" si="35"/>
         <v>4</v>
       </c>
       <c r="C155">
-        <f>$F$150+B155</f>
+        <f t="shared" si="36"/>
         <v>40</v>
       </c>
       <c r="D155">
-        <f>IF(MOD(C155,$B$2)=0,$B$2,MOD(C155,$B$2))</f>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
       <c r="E155">
-        <f>D155*2</f>
+        <f t="shared" si="38"/>
         <v>8</v>
       </c>
       <c r="F155">
-        <f>MOD(E155,$B$3)</f>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
       <c r="H155">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>29</v>
       </c>
       <c r="I155" s="1" t="str">
-        <f>LOOKUP(H155,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" si="41"/>
         <v>T</v>
       </c>
     </row>
@@ -33293,31 +33319,31 @@
         <v>5</v>
       </c>
       <c r="B156" s="1">
-        <f>LOOKUP(A156,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" si="35"/>
         <v>5</v>
       </c>
       <c r="C156">
-        <f>$F$150+B156</f>
+        <f t="shared" si="36"/>
         <v>41</v>
       </c>
       <c r="D156">
-        <f>IF(MOD(C156,$B$2)=0,$B$2,MOD(C156,$B$2))</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
       <c r="E156">
-        <f>D156*2</f>
+        <f t="shared" si="38"/>
         <v>10</v>
       </c>
       <c r="F156">
-        <f>MOD(E156,$B$3)</f>
+        <f t="shared" si="39"/>
         <v>10</v>
       </c>
       <c r="H156">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>27</v>
       </c>
       <c r="I156" s="1" t="str">
-        <f>LOOKUP(H156,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" si="41"/>
         <v>R</v>
       </c>
     </row>
@@ -33326,31 +33352,31 @@
         <v>6</v>
       </c>
       <c r="B157" s="1">
-        <f>LOOKUP(A157,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="C157">
-        <f>$F$150+B157</f>
+        <f t="shared" si="36"/>
         <v>42</v>
       </c>
       <c r="D157">
-        <f>IF(MOD(C157,$B$2)=0,$B$2,MOD(C157,$B$2))</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
       <c r="E157">
-        <f>D157*2</f>
+        <f t="shared" si="38"/>
         <v>12</v>
       </c>
       <c r="F157">
-        <f>MOD(E157,$B$3)</f>
+        <f t="shared" si="39"/>
         <v>12</v>
       </c>
       <c r="H157">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>25</v>
       </c>
       <c r="I157" s="1" t="str">
-        <f>LOOKUP(H157,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" si="41"/>
         <v>P</v>
       </c>
     </row>
@@ -33359,31 +33385,31 @@
         <v>7</v>
       </c>
       <c r="B158" s="1">
-        <f>LOOKUP(A158,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="C158">
-        <f>$F$150+B158</f>
+        <f t="shared" si="36"/>
         <v>43</v>
       </c>
       <c r="D158">
-        <f>IF(MOD(C158,$B$2)=0,$B$2,MOD(C158,$B$2))</f>
+        <f t="shared" si="37"/>
         <v>7</v>
       </c>
       <c r="E158">
-        <f>D158*2</f>
+        <f t="shared" si="38"/>
         <v>14</v>
       </c>
       <c r="F158">
-        <f>MOD(E158,$B$3)</f>
+        <f t="shared" si="39"/>
         <v>14</v>
       </c>
       <c r="H158">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>23</v>
       </c>
       <c r="I158" s="1" t="str">
-        <f>LOOKUP(H158,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" si="41"/>
         <v>N</v>
       </c>
     </row>
@@ -33392,31 +33418,31 @@
         <v>8</v>
       </c>
       <c r="B159" s="1">
-        <f>LOOKUP(A159,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" si="35"/>
         <v>8</v>
       </c>
       <c r="C159">
-        <f>$F$150+B159</f>
+        <f t="shared" si="36"/>
         <v>44</v>
       </c>
       <c r="D159">
-        <f>IF(MOD(C159,$B$2)=0,$B$2,MOD(C159,$B$2))</f>
+        <f t="shared" si="37"/>
         <v>8</v>
       </c>
       <c r="E159">
-        <f>D159*2</f>
+        <f t="shared" si="38"/>
         <v>16</v>
       </c>
       <c r="F159">
-        <f>MOD(E159,$B$3)</f>
+        <f t="shared" si="39"/>
         <v>16</v>
       </c>
       <c r="H159">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>21</v>
       </c>
       <c r="I159" s="1" t="str">
-        <f>LOOKUP(H159,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" si="41"/>
         <v>L</v>
       </c>
     </row>
@@ -33425,31 +33451,31 @@
         <v>9</v>
       </c>
       <c r="B160" s="1">
-        <f>LOOKUP(A160,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" si="35"/>
         <v>9</v>
       </c>
       <c r="C160">
-        <f>$F$150+B160</f>
+        <f t="shared" si="36"/>
         <v>45</v>
       </c>
       <c r="D160">
-        <f>IF(MOD(C160,$B$2)=0,$B$2,MOD(C160,$B$2))</f>
+        <f t="shared" si="37"/>
         <v>9</v>
       </c>
       <c r="E160">
-        <f>D160*2</f>
+        <f t="shared" si="38"/>
         <v>18</v>
       </c>
       <c r="F160">
-        <f>MOD(E160,$B$3)</f>
+        <f t="shared" si="39"/>
         <v>18</v>
       </c>
       <c r="H160">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>19</v>
       </c>
       <c r="I160" s="1" t="str">
-        <f>LOOKUP(H160,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" si="41"/>
         <v>J</v>
       </c>
     </row>
@@ -33458,23 +33484,23 @@
         <v>0</v>
       </c>
       <c r="B161" s="1">
-        <f>LOOKUP(A161,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" si="35"/>
         <v>10</v>
       </c>
       <c r="C161">
-        <f>$F$150+B161</f>
+        <f t="shared" si="36"/>
         <v>46</v>
       </c>
       <c r="D161">
-        <f>IF(MOD(C161,$B$2)=0,$B$2,MOD(C161,$B$2))</f>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="E161">
-        <f>D161*2</f>
+        <f t="shared" si="38"/>
         <v>20</v>
       </c>
       <c r="F161">
-        <f>MOD(E161,$B$3)</f>
+        <f t="shared" si="39"/>
         <v>20</v>
       </c>
       <c r="H161">
@@ -33482,7 +33508,7 @@
         <v>17</v>
       </c>
       <c r="I161" s="1" t="str">
-        <f>LOOKUP(H161,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" si="41"/>
         <v>H</v>
       </c>
     </row>
@@ -33491,31 +33517,31 @@
         <v>1</v>
       </c>
       <c r="B162" s="1">
-        <f t="shared" ref="B162:B186" si="36">LOOKUP(A162,$M$4:$M$39,$N$4:$N$39)</f>
+        <f t="shared" ref="B162:B186" si="42">LOOKUP(A162,$M$4:$M$39,$N$4:$N$39)</f>
         <v>11</v>
       </c>
       <c r="C162">
-        <f t="shared" ref="C162:C186" si="37">$F$150+B162</f>
+        <f t="shared" ref="C162:C186" si="43">$F$150+B162</f>
         <v>47</v>
       </c>
       <c r="D162">
-        <f t="shared" ref="D162:D186" si="38">IF(MOD(C162,$B$2)=0,$B$2,MOD(C162,$B$2))</f>
+        <f t="shared" ref="D162:D186" si="44">IF(MOD(C162,$B$2)=0,$B$2,MOD(C162,$B$2))</f>
         <v>11</v>
       </c>
       <c r="E162">
-        <f t="shared" ref="E162:E186" si="39">D162*2</f>
+        <f t="shared" ref="E162:E186" si="45">D162*2</f>
         <v>22</v>
       </c>
       <c r="F162">
-        <f t="shared" ref="F162:F186" si="40">MOD(E162,$B$3)</f>
+        <f t="shared" ref="F162:F186" si="46">MOD(E162,$B$3)</f>
         <v>22</v>
       </c>
       <c r="H162">
-        <f t="shared" ref="H162:H186" si="41">MOD(($B$2-F162+1),$B$3)</f>
+        <f t="shared" ref="H162:H186" si="47">MOD(($B$2-F162+1),$B$3)</f>
         <v>15</v>
       </c>
       <c r="I162" s="1" t="str">
-        <f t="shared" ref="I162:I186" si="42">LOOKUP(H162,$N$4:$N$39,$M$4:$M$39)</f>
+        <f t="shared" ref="I162:I186" si="48">LOOKUP(H162,$N$4:$N$39,$M$4:$M$39)</f>
         <v>F</v>
       </c>
     </row>
@@ -33524,31 +33550,31 @@
         <v>2</v>
       </c>
       <c r="B163" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>12</v>
       </c>
       <c r="C163">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>48</v>
       </c>
       <c r="D163">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>12</v>
       </c>
       <c r="E163">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>24</v>
       </c>
       <c r="F163">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>24</v>
       </c>
       <c r="H163">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>13</v>
       </c>
       <c r="I163" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>D</v>
       </c>
     </row>
@@ -33557,31 +33583,31 @@
         <v>3</v>
       </c>
       <c r="B164" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>13</v>
       </c>
       <c r="C164">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>49</v>
       </c>
       <c r="D164">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>13</v>
       </c>
       <c r="E164">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>26</v>
       </c>
       <c r="F164">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>26</v>
       </c>
       <c r="H164">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>11</v>
       </c>
       <c r="I164" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>B</v>
       </c>
     </row>
@@ -33590,31 +33616,31 @@
         <v>4</v>
       </c>
       <c r="B165" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>14</v>
       </c>
       <c r="C165">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>50</v>
       </c>
       <c r="D165">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>14</v>
       </c>
       <c r="E165">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>28</v>
       </c>
       <c r="F165">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>28</v>
       </c>
       <c r="H165">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>9</v>
       </c>
       <c r="I165" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>9</v>
       </c>
     </row>
@@ -33623,31 +33649,31 @@
         <v>5</v>
       </c>
       <c r="B166" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>15</v>
       </c>
       <c r="C166">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>51</v>
       </c>
       <c r="D166">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>15</v>
       </c>
       <c r="E166">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>30</v>
       </c>
       <c r="F166">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>30</v>
       </c>
       <c r="H166">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>7</v>
       </c>
       <c r="I166" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>7</v>
       </c>
     </row>
@@ -33656,31 +33682,31 @@
         <v>6</v>
       </c>
       <c r="B167" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>16</v>
       </c>
       <c r="C167">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>52</v>
       </c>
       <c r="D167">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>16</v>
       </c>
       <c r="E167">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>32</v>
       </c>
       <c r="F167">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>32</v>
       </c>
       <c r="H167">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>5</v>
       </c>
       <c r="I167" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>5</v>
       </c>
     </row>
@@ -33689,31 +33715,31 @@
         <v>7</v>
       </c>
       <c r="B168" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>17</v>
       </c>
       <c r="C168">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>53</v>
       </c>
       <c r="D168">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>17</v>
       </c>
       <c r="E168">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>34</v>
       </c>
       <c r="F168">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>34</v>
       </c>
       <c r="H168">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>3</v>
       </c>
       <c r="I168" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>3</v>
       </c>
     </row>
@@ -33722,31 +33748,31 @@
         <v>8</v>
       </c>
       <c r="B169" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>18</v>
       </c>
       <c r="C169">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>54</v>
       </c>
       <c r="D169">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>18</v>
       </c>
       <c r="E169">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>36</v>
       </c>
       <c r="F169">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>36</v>
       </c>
       <c r="H169">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="I169" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>1</v>
       </c>
     </row>
@@ -33755,31 +33781,31 @@
         <v>9</v>
       </c>
       <c r="B170" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>19</v>
       </c>
       <c r="C170">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>55</v>
       </c>
       <c r="D170">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>19</v>
       </c>
       <c r="E170">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>38</v>
       </c>
       <c r="F170">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>1</v>
       </c>
       <c r="H170">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>36</v>
       </c>
       <c r="I170" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>Z</v>
       </c>
       <c r="J170" t="s">
@@ -33791,31 +33817,31 @@
         <v>10</v>
       </c>
       <c r="B171" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>20</v>
       </c>
       <c r="C171">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>56</v>
       </c>
       <c r="D171">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>20</v>
       </c>
       <c r="E171">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>40</v>
       </c>
       <c r="F171">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>3</v>
       </c>
       <c r="H171">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>34</v>
       </c>
       <c r="I171" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>Y</v>
       </c>
     </row>
@@ -33824,31 +33850,31 @@
         <v>11</v>
       </c>
       <c r="B172" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>21</v>
       </c>
       <c r="C172">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>57</v>
       </c>
       <c r="D172">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>21</v>
       </c>
       <c r="E172">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>42</v>
       </c>
       <c r="F172">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>5</v>
       </c>
       <c r="H172">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>32</v>
       </c>
       <c r="I172" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>W</v>
       </c>
     </row>
@@ -33857,31 +33883,31 @@
         <v>12</v>
       </c>
       <c r="B173" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>22</v>
       </c>
       <c r="C173">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>58</v>
       </c>
       <c r="D173">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>22</v>
       </c>
       <c r="E173">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>44</v>
       </c>
       <c r="F173">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>7</v>
       </c>
       <c r="H173">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>30</v>
       </c>
       <c r="I173" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>U</v>
       </c>
     </row>
@@ -33890,31 +33916,31 @@
         <v>13</v>
       </c>
       <c r="B174" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>23</v>
       </c>
       <c r="C174">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>59</v>
       </c>
       <c r="D174">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>23</v>
       </c>
       <c r="E174">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>46</v>
       </c>
       <c r="F174">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>9</v>
       </c>
       <c r="H174">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>28</v>
       </c>
       <c r="I174" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>S</v>
       </c>
     </row>
@@ -33923,31 +33949,31 @@
         <v>14</v>
       </c>
       <c r="B175" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>24</v>
       </c>
       <c r="C175">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>60</v>
       </c>
       <c r="D175">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>24</v>
       </c>
       <c r="E175">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>48</v>
       </c>
       <c r="F175">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>11</v>
       </c>
       <c r="H175">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>26</v>
       </c>
       <c r="I175" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>Q</v>
       </c>
     </row>
@@ -33956,31 +33982,31 @@
         <v>15</v>
       </c>
       <c r="B176" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>25</v>
       </c>
       <c r="C176">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>61</v>
       </c>
       <c r="D176">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>25</v>
       </c>
       <c r="E176">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>50</v>
       </c>
       <c r="F176">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>13</v>
       </c>
       <c r="H176">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>24</v>
       </c>
       <c r="I176" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>O</v>
       </c>
     </row>
@@ -33989,31 +34015,31 @@
         <v>16</v>
       </c>
       <c r="B177" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>26</v>
       </c>
       <c r="C177">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>62</v>
       </c>
       <c r="D177">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>26</v>
       </c>
       <c r="E177">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>52</v>
       </c>
       <c r="F177">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>15</v>
       </c>
       <c r="H177">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>22</v>
       </c>
       <c r="I177" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>M</v>
       </c>
     </row>
@@ -34022,31 +34048,31 @@
         <v>17</v>
       </c>
       <c r="B178" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>27</v>
       </c>
       <c r="C178">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>63</v>
       </c>
       <c r="D178">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>27</v>
       </c>
       <c r="E178">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>54</v>
       </c>
       <c r="F178">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>17</v>
       </c>
       <c r="H178">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>20</v>
       </c>
       <c r="I178" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>K</v>
       </c>
     </row>
@@ -34055,31 +34081,31 @@
         <v>18</v>
       </c>
       <c r="B179" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>28</v>
       </c>
       <c r="C179">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>64</v>
       </c>
       <c r="D179">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>28</v>
       </c>
       <c r="E179">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>56</v>
       </c>
       <c r="F179">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>19</v>
       </c>
       <c r="H179">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>18</v>
       </c>
       <c r="I179" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>I</v>
       </c>
     </row>
@@ -34088,31 +34114,31 @@
         <v>19</v>
       </c>
       <c r="B180" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>29</v>
       </c>
       <c r="C180">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>65</v>
       </c>
       <c r="D180">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>29</v>
       </c>
       <c r="E180">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>58</v>
       </c>
       <c r="F180">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>21</v>
       </c>
       <c r="H180">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>16</v>
       </c>
       <c r="I180" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>G</v>
       </c>
     </row>
@@ -34121,31 +34147,31 @@
         <v>20</v>
       </c>
       <c r="B181" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>30</v>
       </c>
       <c r="C181">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>66</v>
       </c>
       <c r="D181">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>30</v>
       </c>
       <c r="E181">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>60</v>
       </c>
       <c r="F181">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>23</v>
       </c>
       <c r="H181">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>14</v>
       </c>
       <c r="I181" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>E</v>
       </c>
     </row>
@@ -34154,31 +34180,31 @@
         <v>21</v>
       </c>
       <c r="B182" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>31</v>
       </c>
       <c r="C182">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>67</v>
       </c>
       <c r="D182">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>31</v>
       </c>
       <c r="E182">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>62</v>
       </c>
       <c r="F182">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>25</v>
       </c>
       <c r="H182">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>12</v>
       </c>
       <c r="I182" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>C</v>
       </c>
     </row>
@@ -34187,31 +34213,31 @@
         <v>22</v>
       </c>
       <c r="B183" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>32</v>
       </c>
       <c r="C183">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>68</v>
       </c>
       <c r="D183">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>32</v>
       </c>
       <c r="E183">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>64</v>
       </c>
       <c r="F183">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>27</v>
       </c>
       <c r="H183">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>10</v>
       </c>
       <c r="I183" s="1" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>A</v>
       </c>
     </row>
@@ -34220,31 +34246,31 @@
         <v>23</v>
       </c>
       <c r="B184" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>33</v>
       </c>
       <c r="C184">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>69</v>
       </c>
       <c r="D184">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>33</v>
       </c>
       <c r="E184">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>66</v>
       </c>
       <c r="F184">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>29</v>
       </c>
       <c r="H184">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>8</v>
       </c>
       <c r="I184" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>8</v>
       </c>
     </row>
@@ -34253,31 +34279,31 @@
         <v>53</v>
       </c>
       <c r="B185" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>34</v>
       </c>
       <c r="C185">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>70</v>
       </c>
       <c r="D185">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>34</v>
       </c>
       <c r="E185">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>68</v>
       </c>
       <c r="F185">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>31</v>
       </c>
       <c r="H185">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>6</v>
       </c>
       <c r="I185" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>6</v>
       </c>
     </row>
@@ -34286,60 +34312,656 @@
         <v>24</v>
       </c>
       <c r="B186" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>35</v>
       </c>
       <c r="C186">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>71</v>
       </c>
       <c r="D186">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>35</v>
       </c>
       <c r="E186">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>70</v>
       </c>
       <c r="F186">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>33</v>
       </c>
       <c r="H186">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>4</v>
       </c>
       <c r="I186" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="48"/>
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C12:C16 C151:C186">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C36">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C65">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74:C109">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C118:C143">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5BABD-809B-47ED-BCA9-0B303830648B}">
+  <dimension ref="A1:O40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="10.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1">
+        <f>TRUNC(2147483647/B3)</f>
+        <v>1073741823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1">
+        <f>LOOKUP(A11,$N$11:$N$40,$O$11:$O$40)</f>
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <f>(C10+B11)*$B$3</f>
+        <v>36</v>
+      </c>
+      <c r="D11">
+        <f>MOD((D10+B11)*$B$3,$B$2)</f>
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <f>MOD(D11*$B$3,$B$2)</f>
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <f>$B$2+1-F11</f>
+        <v>16</v>
+      </c>
+      <c r="H11">
+        <f>(G11-I11)/$B$3</f>
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <f>MOD(G11,$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="str">
+        <f>LOOKUP(H11,$O$11:$O$39,$N$11:$N$39)</f>
+        <v>I</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f>LOOKUP(I11,$O$11:$O$39,$N$11:$N$39)</f>
+        <v>A</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="1">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C16" si="0">(C11+B12)*$B$3</f>
+        <v>126</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:D16" si="1">MOD((D11+B12)*$B$3,$B$2)</f>
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F16" si="2">MOD(D12*$B$3,$B$2)</f>
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G16" si="3">$B$2+1-F12</f>
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ref="H12:H16" si="4">(G12-I12)/$B$3</f>
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I16" si="5">MOD(G12,$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="str">
+        <f t="shared" ref="J12:J16" si="6">LOOKUP(H12,$O$11:$O$39,$N$11:$N$39)</f>
+        <v>F</v>
+      </c>
+      <c r="K12" s="1" t="str">
+        <f t="shared" ref="K12:K16" si="7">LOOKUP(I12,$O$11:$O$39,$N$11:$N$39)</f>
+        <v>A</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1">
+        <f>LOOKUP(A13,$N$11:$N$40,$O$11:$O$40)</f>
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>288</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>C</v>
+      </c>
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>B</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1">
+        <f>LOOKUP(A14,$N$11:$N$40,$O$11:$O$40)</f>
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>614</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>K</v>
+      </c>
+      <c r="K14" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>A</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <f>LOOKUP(A15,$N$11:$N$40,$O$11:$O$40)</f>
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1236</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>L</v>
+      </c>
+      <c r="K15" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>B</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <f>LOOKUP(A16,$N$11:$N$40,$O$11:$O$40)</f>
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>2506</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>D</v>
+      </c>
+      <c r="K16" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>A</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O16" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="N17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="N18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O19" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O20" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O21" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O22" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O24" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O26" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O28" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O29" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O30" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O31" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O32" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O33" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O34" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O35" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O36" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N37" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O37" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O38" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O39" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O40" s="1">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C11:C16">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>$B$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
IbanAlgorithm implementation and associated unit tests. Plus fix minor copy and paste error in some ISO tests
</commit_message>
<xml_diff>
--- a/Documentation/ISO7064ExamplesWorkbook.xlsx
+++ b/Documentation/ISO7064ExamplesWorkbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CheckDigits.Net\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A947603-616F-4C3D-9580-BB40B1F7A621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E5CD4E-68A6-4DFA-B508-7A68B1DB21F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="7" xr2:uid="{29668144-CB59-4756-8844-303BE2B9F3CC}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{29668144-CB59-4756-8844-303BE2B9F3CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="90">
   <si>
     <t>A</t>
   </si>
@@ -311,6 +311,9 @@
   <si>
     <t>OSlash</t>
   </si>
+  <si>
+    <t>IBAN mapping</t>
+  </si>
 </sst>
 </file>
 
@@ -389,7 +392,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -13947,60 +13990,60 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C17">
-    <cfRule type="cellIs" dxfId="43" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="13" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C38">
-    <cfRule type="cellIs" dxfId="42" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="7" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="8" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C59">
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="5" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67:C102">
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="3" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C109:C144">
-    <cfRule type="cellIs" dxfId="36" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="9" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152:C187">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:F61">
-    <cfRule type="cellIs" dxfId="33" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="12" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="16" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F103">
-    <cfRule type="cellIs" dxfId="31" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="11" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="15" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19537,31 +19580,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C17 C140:C165">
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="8" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C38">
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="7" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C59">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="5" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C91 C97:C134">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19571,10 +19614,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF67E24C-1E84-413B-9210-17598F74D757}">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22289,21 +22332,262 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>0</v>
+      </c>
+      <c r="B111" s="1">
+        <v>3</v>
+      </c>
+      <c r="C111">
+        <f>(C110+B111)*$B$3</f>
+        <v>30</v>
+      </c>
+      <c r="D111">
+        <f>MOD((D110+B111)*$B$3,$B$2)</f>
+        <v>30</v>
+      </c>
+      <c r="F111">
+        <f>MOD(D111*$B$3,$B$2)</f>
+        <v>9</v>
+      </c>
+      <c r="G111" s="1">
+        <f>$B$2+1-F111</f>
+        <v>89</v>
+      </c>
+      <c r="H111" s="1">
+        <f>(G111-I111)/$B$3</f>
+        <v>8</v>
+      </c>
+      <c r="I111">
+        <f>MOD(G111,$B$3)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>1</v>
+      </c>
+      <c r="B112" s="1">
+        <v>2</v>
+      </c>
+      <c r="C112">
+        <f t="shared" ref="C112:C115" si="42">(C111+B112)*$B$3</f>
+        <v>320</v>
+      </c>
+      <c r="D112">
+        <f t="shared" ref="D112:D115" si="43">MOD((D111+B112)*$B$3,$B$2)</f>
+        <v>29</v>
+      </c>
+      <c r="F112">
+        <f t="shared" ref="F112:F115" si="44">MOD(D112*$B$3,$B$2)</f>
+        <v>96</v>
+      </c>
+      <c r="G112" s="1">
+        <f t="shared" ref="G112:G116" si="45">$B$2+1-F112</f>
+        <v>2</v>
+      </c>
+      <c r="H112" s="1">
+        <f t="shared" ref="H112:H116" si="46">(G112-I112)/$B$3</f>
+        <v>0</v>
+      </c>
+      <c r="I112">
+        <f t="shared" ref="I112:I115" si="47">MOD(G112,$B$3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>0</v>
+      </c>
+      <c r="B113" s="1">
+        <v>1</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="42"/>
+        <v>3210</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="43"/>
+        <v>9</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="44"/>
+        <v>90</v>
+      </c>
+      <c r="G113" s="1">
+        <f t="shared" si="45"/>
+        <v>8</v>
+      </c>
+      <c r="H113" s="1">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="I113">
+        <f t="shared" si="47"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>1</v>
+      </c>
+      <c r="B114" s="1">
+        <v>0</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="42"/>
+        <v>32100</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="43"/>
+        <v>90</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="44"/>
+        <v>27</v>
+      </c>
+      <c r="G114" s="1">
+        <f t="shared" si="45"/>
+        <v>71</v>
+      </c>
+      <c r="H114" s="1">
+        <f t="shared" si="46"/>
+        <v>7</v>
+      </c>
+      <c r="I114">
+        <f t="shared" si="47"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>0</v>
+      </c>
+      <c r="B115" s="1">
+        <v>1</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="42"/>
+        <v>321010</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="43"/>
+        <v>37</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="44"/>
+        <v>79</v>
+      </c>
+      <c r="G115" s="1">
+        <f t="shared" si="45"/>
+        <v>19</v>
+      </c>
+      <c r="H115" s="1">
+        <f t="shared" si="46"/>
+        <v>1</v>
+      </c>
+      <c r="I115">
+        <f t="shared" si="47"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="1">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <f t="shared" ref="C116" si="48">(C115+B116)*$B$3</f>
+        <v>3210100</v>
+      </c>
+      <c r="D116">
+        <f t="shared" ref="D116" si="49">MOD((D115+B116)*$B$3,$B$2)</f>
+        <v>79</v>
+      </c>
+      <c r="F116">
+        <f t="shared" ref="F116" si="50">MOD(D116*$B$3,$B$2)</f>
+        <v>14</v>
+      </c>
+      <c r="G116" s="1">
+        <f t="shared" si="45"/>
+        <v>84</v>
+      </c>
+      <c r="H116" s="1">
+        <f t="shared" si="46"/>
+        <v>8</v>
+      </c>
+      <c r="I116">
+        <f t="shared" ref="I116" si="51">MOD(G116,$B$3)</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C18 C94:C103">
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="11" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C41">
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C88">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="greaterThan">
+      <formula>$B$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C111:C116">
     <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
@@ -34374,7 +34658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5BABD-809B-47ED-BCA9-0B303830648B}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
AlphanumericMod97_10Algorithm implementation and unit tests
</commit_message>
<xml_diff>
--- a/Documentation/ISO7064ExamplesWorkbook.xlsx
+++ b/Documentation/ISO7064ExamplesWorkbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CheckDigits.Net\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E5CD4E-68A6-4DFA-B508-7A68B1DB21F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A20487-4AB1-4E78-9B6B-86BB45230EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{29668144-CB59-4756-8844-303BE2B9F3CC}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="91">
   <si>
     <t>A</t>
   </si>
@@ -314,6 +314,9 @@
   <si>
     <t>IBAN mapping</t>
   </si>
+  <si>
+    <t>Additional values for Alphanumeric Mod 97-10</t>
+  </si>
 </sst>
 </file>
 
@@ -392,27 +395,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="46">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -13990,60 +13973,60 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C17">
-    <cfRule type="cellIs" dxfId="47" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="13" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C38">
-    <cfRule type="cellIs" dxfId="46" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="7" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="8" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C59">
-    <cfRule type="cellIs" dxfId="44" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67:C102">
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="3" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C109:C144">
-    <cfRule type="cellIs" dxfId="40" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="9" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C152:C187">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F60:F61">
-    <cfRule type="cellIs" dxfId="37" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="12" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="16" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F103">
-    <cfRule type="cellIs" dxfId="35" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="11" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="15" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14056,8 +14039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A402F48E-7D2E-4A97-B8F3-3C3001D1588A}">
   <dimension ref="A1:O165"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:K17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13:N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19580,31 +19563,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C13:C17 C140:C165">
-    <cfRule type="cellIs" dxfId="33" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C38">
-    <cfRule type="cellIs" dxfId="32" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C59">
-    <cfRule type="cellIs" dxfId="30" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C91 C97:C134">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19614,10 +19597,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF67E24C-1E84-413B-9210-17598F74D757}">
-  <dimension ref="A1:M116"/>
+  <dimension ref="A1:M144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="I107" sqref="I107:I132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22332,262 +22315,1156 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
     </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="J104" s="1"/>
+      <c r="K104" s="1"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="J106" s="1"/>
+      <c r="K106" s="1"/>
+    </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="A107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107" s="1">
+        <v>10</v>
+      </c>
+      <c r="C107">
+        <f t="shared" ref="C107" si="42">B107*$B$3</f>
+        <v>100</v>
+      </c>
+      <c r="D107">
+        <f t="shared" ref="D107" si="43">MOD(B107*$B$3,$B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="F107">
+        <f t="shared" ref="F107" si="44">MOD(D107*$B$3,$B$2)</f>
+        <v>30</v>
+      </c>
+      <c r="G107" s="1">
+        <f t="shared" ref="G107" si="45">$B$2+1-F107</f>
+        <v>68</v>
+      </c>
+      <c r="H107" s="1">
+        <f t="shared" ref="H107" si="46">(G107-I107)/$B$3</f>
+        <v>6</v>
+      </c>
+      <c r="I107">
+        <f t="shared" ref="I107" si="47">MOD(G107,$B$3)</f>
+        <v>8</v>
+      </c>
+      <c r="J107" s="1"/>
+      <c r="K107" s="1"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B108" s="1">
+        <v>11</v>
+      </c>
+      <c r="C108">
+        <f t="shared" ref="C108:C132" si="48">B108*$B$3</f>
+        <v>110</v>
+      </c>
+      <c r="D108">
+        <f t="shared" ref="D108:D132" si="49">MOD(B108*$B$3,$B$2)</f>
+        <v>13</v>
+      </c>
+      <c r="F108">
+        <f t="shared" ref="F108:F132" si="50">MOD(D108*$B$3,$B$2)</f>
+        <v>33</v>
+      </c>
+      <c r="G108" s="1">
+        <f t="shared" ref="G108:G132" si="51">$B$2+1-F108</f>
+        <v>65</v>
+      </c>
+      <c r="H108" s="1">
+        <f t="shared" ref="H108:H132" si="52">(G108-I108)/$B$3</f>
+        <v>6</v>
+      </c>
+      <c r="I108">
+        <f t="shared" ref="I108:I132" si="53">MOD(G108,$B$3)</f>
+        <v>5</v>
+      </c>
+      <c r="J108" s="1"/>
+      <c r="K108" s="1"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="1">
+        <v>12</v>
+      </c>
+      <c r="C109">
+        <f t="shared" si="48"/>
+        <v>120</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="49"/>
+        <v>23</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="50"/>
+        <v>36</v>
+      </c>
+      <c r="G109" s="1">
+        <f t="shared" si="51"/>
+        <v>62</v>
+      </c>
+      <c r="H109" s="1">
+        <f t="shared" si="52"/>
+        <v>6</v>
+      </c>
+      <c r="I109">
+        <f t="shared" si="53"/>
+        <v>2</v>
+      </c>
+      <c r="J109" s="1"/>
+      <c r="K109" s="1"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" s="1">
+        <v>13</v>
+      </c>
+      <c r="C110">
+        <f t="shared" si="48"/>
+        <v>130</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="49"/>
+        <v>33</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="50"/>
+        <v>39</v>
+      </c>
+      <c r="G110" s="1">
+        <f t="shared" si="51"/>
+        <v>59</v>
+      </c>
+      <c r="H110" s="1">
+        <f t="shared" si="52"/>
+        <v>5</v>
+      </c>
+      <c r="I110">
+        <f t="shared" si="53"/>
+        <v>9</v>
+      </c>
+      <c r="J110" s="1"/>
+      <c r="K110" s="1"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" s="1">
+        <v>14</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="48"/>
+        <v>140</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="49"/>
+        <v>43</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="50"/>
+        <v>42</v>
+      </c>
+      <c r="G111" s="1">
+        <f t="shared" si="51"/>
+        <v>56</v>
+      </c>
+      <c r="H111" s="1">
+        <f t="shared" si="52"/>
+        <v>5</v>
+      </c>
+      <c r="I111">
+        <f t="shared" si="53"/>
+        <v>6</v>
+      </c>
+      <c r="J111" s="1"/>
+      <c r="K111" s="1"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" s="1">
+        <v>15</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="48"/>
+        <v>150</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="49"/>
+        <v>53</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="50"/>
+        <v>45</v>
+      </c>
+      <c r="G112" s="1">
+        <f t="shared" si="51"/>
+        <v>53</v>
+      </c>
+      <c r="H112" s="1">
+        <f t="shared" si="52"/>
+        <v>5</v>
+      </c>
+      <c r="I112">
+        <f t="shared" si="53"/>
+        <v>3</v>
+      </c>
+      <c r="J112" s="1"/>
+      <c r="K112" s="1"/>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113" s="1">
+        <v>16</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="48"/>
+        <v>160</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="49"/>
+        <v>63</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="50"/>
+        <v>48</v>
+      </c>
+      <c r="G113" s="1">
+        <f t="shared" si="51"/>
+        <v>50</v>
+      </c>
+      <c r="H113" s="1">
+        <f t="shared" si="52"/>
+        <v>5</v>
+      </c>
+      <c r="I113">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="J113" s="1"/>
+      <c r="K113" s="1"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B114" s="1">
+        <v>17</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="48"/>
+        <v>170</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="49"/>
+        <v>73</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="50"/>
+        <v>51</v>
+      </c>
+      <c r="G114" s="1">
+        <f t="shared" si="51"/>
+        <v>47</v>
+      </c>
+      <c r="H114" s="1">
+        <f t="shared" si="52"/>
+        <v>4</v>
+      </c>
+      <c r="I114">
+        <f t="shared" si="53"/>
+        <v>7</v>
+      </c>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B115" s="1">
+        <v>18</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="48"/>
+        <v>180</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="49"/>
+        <v>83</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="50"/>
+        <v>54</v>
+      </c>
+      <c r="G115" s="1">
+        <f t="shared" si="51"/>
+        <v>44</v>
+      </c>
+      <c r="H115" s="1">
+        <f t="shared" si="52"/>
+        <v>4</v>
+      </c>
+      <c r="I115">
+        <f t="shared" si="53"/>
+        <v>4</v>
+      </c>
+      <c r="J115" s="1"/>
+      <c r="K115" s="1"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B116" s="1">
+        <v>19</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="48"/>
+        <v>190</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="49"/>
+        <v>93</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="50"/>
+        <v>57</v>
+      </c>
+      <c r="G116" s="1">
+        <f t="shared" si="51"/>
+        <v>41</v>
+      </c>
+      <c r="H116" s="1">
+        <f t="shared" si="52"/>
+        <v>4</v>
+      </c>
+      <c r="I116">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="J116" s="1"/>
+      <c r="K116" s="1"/>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B117" s="1">
+        <v>20</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="48"/>
+        <v>200</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="49"/>
+        <v>6</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="50"/>
+        <v>60</v>
+      </c>
+      <c r="G117" s="1">
+        <f t="shared" si="51"/>
+        <v>38</v>
+      </c>
+      <c r="H117" s="1">
+        <f t="shared" si="52"/>
+        <v>3</v>
+      </c>
+      <c r="I117">
+        <f t="shared" si="53"/>
+        <v>8</v>
+      </c>
+      <c r="J117" s="1"/>
+      <c r="K117" s="1"/>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B118" s="1">
+        <v>21</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="48"/>
+        <v>210</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="49"/>
+        <v>16</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="50"/>
+        <v>63</v>
+      </c>
+      <c r="G118" s="1">
+        <f t="shared" si="51"/>
+        <v>35</v>
+      </c>
+      <c r="H118" s="1">
+        <f t="shared" si="52"/>
+        <v>3</v>
+      </c>
+      <c r="I118">
+        <f t="shared" si="53"/>
+        <v>5</v>
+      </c>
+      <c r="J118" s="1"/>
+      <c r="K118" s="1"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B119" s="1">
+        <v>22</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="48"/>
+        <v>220</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="49"/>
+        <v>26</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="50"/>
+        <v>66</v>
+      </c>
+      <c r="G119" s="1">
+        <f t="shared" si="51"/>
+        <v>32</v>
+      </c>
+      <c r="H119" s="1">
+        <f t="shared" si="52"/>
+        <v>3</v>
+      </c>
+      <c r="I119">
+        <f t="shared" si="53"/>
+        <v>2</v>
+      </c>
+      <c r="J119" s="1"/>
+      <c r="K119" s="1"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B120" s="1">
+        <v>23</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="48"/>
+        <v>230</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="49"/>
+        <v>36</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="50"/>
+        <v>69</v>
+      </c>
+      <c r="G120" s="1">
+        <f t="shared" si="51"/>
+        <v>29</v>
+      </c>
+      <c r="H120" s="1">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="I120">
+        <f t="shared" si="53"/>
+        <v>9</v>
+      </c>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B121" s="1">
+        <v>24</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="48"/>
+        <v>240</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="49"/>
+        <v>46</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="50"/>
+        <v>72</v>
+      </c>
+      <c r="G121" s="1">
+        <f t="shared" si="51"/>
+        <v>26</v>
+      </c>
+      <c r="H121" s="1">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="I121">
+        <f t="shared" si="53"/>
+        <v>6</v>
+      </c>
+      <c r="J121" s="1"/>
+      <c r="K121" s="1"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B122" s="1">
+        <v>25</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="48"/>
+        <v>250</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="49"/>
+        <v>56</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="50"/>
+        <v>75</v>
+      </c>
+      <c r="G122" s="1">
+        <f t="shared" si="51"/>
+        <v>23</v>
+      </c>
+      <c r="H122" s="1">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="I122">
+        <f t="shared" si="53"/>
+        <v>3</v>
+      </c>
+      <c r="J122" s="1"/>
+      <c r="K122" s="1"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B123" s="1">
+        <v>26</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="48"/>
+        <v>260</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="49"/>
+        <v>66</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="50"/>
+        <v>78</v>
+      </c>
+      <c r="G123" s="1">
+        <f t="shared" si="51"/>
+        <v>20</v>
+      </c>
+      <c r="H123" s="1">
+        <f t="shared" si="52"/>
+        <v>2</v>
+      </c>
+      <c r="I123">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="J123" s="1"/>
+      <c r="K123" s="1"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B124" s="1">
+        <v>27</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="48"/>
+        <v>270</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="49"/>
+        <v>76</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="50"/>
+        <v>81</v>
+      </c>
+      <c r="G124" s="1">
+        <f t="shared" si="51"/>
+        <v>17</v>
+      </c>
+      <c r="H124" s="1">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="I124">
+        <f t="shared" si="53"/>
+        <v>7</v>
+      </c>
+      <c r="J124" s="1"/>
+      <c r="K124" s="1"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B125" s="1">
+        <v>28</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="48"/>
+        <v>280</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="49"/>
+        <v>86</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="50"/>
+        <v>84</v>
+      </c>
+      <c r="G125" s="1">
+        <f t="shared" si="51"/>
+        <v>14</v>
+      </c>
+      <c r="H125" s="1">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="I125">
+        <f t="shared" si="53"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B126" s="1">
+        <v>29</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="48"/>
+        <v>290</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="49"/>
+        <v>96</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="50"/>
+        <v>87</v>
+      </c>
+      <c r="G126" s="1">
+        <f t="shared" si="51"/>
+        <v>11</v>
+      </c>
+      <c r="H126" s="1">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="I126">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B127" s="1">
+        <v>30</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="48"/>
+        <v>300</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="49"/>
+        <v>9</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="50"/>
+        <v>90</v>
+      </c>
+      <c r="G127" s="1">
+        <f t="shared" si="51"/>
+        <v>8</v>
+      </c>
+      <c r="H127" s="1">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="I127">
+        <f t="shared" si="53"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B128" s="1">
+        <v>31</v>
+      </c>
+      <c r="C128">
+        <f t="shared" si="48"/>
+        <v>310</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="49"/>
+        <v>19</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="50"/>
+        <v>93</v>
+      </c>
+      <c r="G128" s="1">
+        <f t="shared" si="51"/>
+        <v>5</v>
+      </c>
+      <c r="H128" s="1">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="I128">
+        <f t="shared" si="53"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B129" s="1">
+        <v>32</v>
+      </c>
+      <c r="C129">
+        <f t="shared" si="48"/>
+        <v>320</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="49"/>
+        <v>29</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="50"/>
+        <v>96</v>
+      </c>
+      <c r="G129" s="1">
+        <f t="shared" si="51"/>
+        <v>2</v>
+      </c>
+      <c r="H129" s="1">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="I129">
+        <f t="shared" si="53"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B130" s="1">
+        <v>33</v>
+      </c>
+      <c r="C130">
+        <f t="shared" si="48"/>
+        <v>330</v>
+      </c>
+      <c r="D130">
+        <f t="shared" si="49"/>
+        <v>39</v>
+      </c>
+      <c r="F130">
+        <f t="shared" si="50"/>
+        <v>2</v>
+      </c>
+      <c r="G130" s="1">
+        <f t="shared" si="51"/>
+        <v>96</v>
+      </c>
+      <c r="H130" s="1">
+        <f t="shared" si="52"/>
+        <v>9</v>
+      </c>
+      <c r="I130">
+        <f t="shared" si="53"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B131" s="1">
+        <v>34</v>
+      </c>
+      <c r="C131">
+        <f t="shared" si="48"/>
+        <v>340</v>
+      </c>
+      <c r="D131">
+        <f t="shared" si="49"/>
+        <v>49</v>
+      </c>
+      <c r="F131">
+        <f t="shared" si="50"/>
+        <v>5</v>
+      </c>
+      <c r="G131" s="1">
+        <f t="shared" si="51"/>
+        <v>93</v>
+      </c>
+      <c r="H131" s="1">
+        <f t="shared" si="52"/>
+        <v>9</v>
+      </c>
+      <c r="I131">
+        <f t="shared" si="53"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B132" s="1">
+        <v>35</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="48"/>
+        <v>350</v>
+      </c>
+      <c r="D132">
+        <f t="shared" si="49"/>
+        <v>59</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="50"/>
+        <v>8</v>
+      </c>
+      <c r="G132" s="1">
+        <f t="shared" si="51"/>
+        <v>90</v>
+      </c>
+      <c r="H132" s="1">
+        <f t="shared" si="52"/>
+        <v>9</v>
+      </c>
+      <c r="I132">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="3" t="s">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="D137" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-      <c r="I109" s="1"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+      <c r="G137" s="1"/>
+      <c r="H137" s="1"/>
+      <c r="I137" s="1"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B138" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C110">
+      <c r="C138">
         <v>0</v>
       </c>
-      <c r="D110">
+      <c r="D138">
         <v>0</v>
       </c>
-      <c r="F110" s="3" t="s">
+      <c r="F138" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G110" s="2" t="s">
+      <c r="G138" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H110" s="2" t="s">
+      <c r="H138" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I110" s="3" t="s">
+      <c r="I138" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
         <v>0</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B139" s="1">
         <v>3</v>
       </c>
-      <c r="C111">
-        <f>(C110+B111)*$B$3</f>
+      <c r="C139">
+        <f>(C138+B139)*$B$3</f>
         <v>30</v>
       </c>
-      <c r="D111">
-        <f>MOD((D110+B111)*$B$3,$B$2)</f>
+      <c r="D139">
+        <f>MOD((D138+B139)*$B$3,$B$2)</f>
         <v>30</v>
       </c>
-      <c r="F111">
-        <f>MOD(D111*$B$3,$B$2)</f>
+      <c r="F139">
+        <f>MOD(D139*$B$3,$B$2)</f>
         <v>9</v>
       </c>
-      <c r="G111" s="1">
-        <f>$B$2+1-F111</f>
+      <c r="G139" s="1">
+        <f>$B$2+1-F139</f>
         <v>89</v>
       </c>
-      <c r="H111" s="1">
-        <f>(G111-I111)/$B$3</f>
+      <c r="H139" s="1">
+        <f>(G139-I139)/$B$3</f>
         <v>8</v>
       </c>
-      <c r="I111">
-        <f>MOD(G111,$B$3)</f>
+      <c r="I139">
+        <f>MOD(G139,$B$3)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
         <v>1</v>
       </c>
-      <c r="B112" s="1">
-        <v>2</v>
-      </c>
-      <c r="C112">
-        <f t="shared" ref="C112:C115" si="42">(C111+B112)*$B$3</f>
+      <c r="B140" s="1">
+        <v>2</v>
+      </c>
+      <c r="C140">
+        <f t="shared" ref="C140:C143" si="54">(C139+B140)*$B$3</f>
         <v>320</v>
       </c>
-      <c r="D112">
-        <f t="shared" ref="D112:D115" si="43">MOD((D111+B112)*$B$3,$B$2)</f>
+      <c r="D140">
+        <f t="shared" ref="D140:D143" si="55">MOD((D139+B140)*$B$3,$B$2)</f>
         <v>29</v>
       </c>
-      <c r="F112">
-        <f t="shared" ref="F112:F115" si="44">MOD(D112*$B$3,$B$2)</f>
+      <c r="F140">
+        <f t="shared" ref="F140:F143" si="56">MOD(D140*$B$3,$B$2)</f>
         <v>96</v>
       </c>
-      <c r="G112" s="1">
-        <f t="shared" ref="G112:G116" si="45">$B$2+1-F112</f>
-        <v>2</v>
-      </c>
-      <c r="H112" s="1">
-        <f t="shared" ref="H112:H116" si="46">(G112-I112)/$B$3</f>
+      <c r="G140" s="1">
+        <f t="shared" ref="G140:G144" si="57">$B$2+1-F140</f>
+        <v>2</v>
+      </c>
+      <c r="H140" s="1">
+        <f t="shared" ref="H140:H144" si="58">(G140-I140)/$B$3</f>
         <v>0</v>
       </c>
-      <c r="I112">
-        <f t="shared" ref="I112:I115" si="47">MOD(G112,$B$3)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
+      <c r="I140">
+        <f t="shared" ref="I140:I143" si="59">MOD(G140,$B$3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
         <v>0</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B141" s="1">
         <v>1</v>
       </c>
-      <c r="C113">
-        <f t="shared" si="42"/>
+      <c r="C141">
+        <f t="shared" si="54"/>
         <v>3210</v>
       </c>
-      <c r="D113">
-        <f t="shared" si="43"/>
+      <c r="D141">
+        <f t="shared" si="55"/>
         <v>9</v>
       </c>
-      <c r="F113">
-        <f t="shared" si="44"/>
+      <c r="F141">
+        <f t="shared" si="56"/>
         <v>90</v>
       </c>
-      <c r="G113" s="1">
-        <f t="shared" si="45"/>
+      <c r="G141" s="1">
+        <f t="shared" si="57"/>
         <v>8</v>
       </c>
-      <c r="H113" s="1">
-        <f t="shared" si="46"/>
+      <c r="H141" s="1">
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="I113">
-        <f t="shared" si="47"/>
+      <c r="I141">
+        <f t="shared" si="59"/>
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
         <v>1</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B142" s="1">
         <v>0</v>
       </c>
-      <c r="C114">
-        <f t="shared" si="42"/>
+      <c r="C142">
+        <f t="shared" si="54"/>
         <v>32100</v>
       </c>
-      <c r="D114">
-        <f t="shared" si="43"/>
+      <c r="D142">
+        <f t="shared" si="55"/>
         <v>90</v>
       </c>
-      <c r="F114">
-        <f t="shared" si="44"/>
+      <c r="F142">
+        <f t="shared" si="56"/>
         <v>27</v>
       </c>
-      <c r="G114" s="1">
-        <f t="shared" si="45"/>
+      <c r="G142" s="1">
+        <f t="shared" si="57"/>
         <v>71</v>
       </c>
-      <c r="H114" s="1">
-        <f t="shared" si="46"/>
+      <c r="H142" s="1">
+        <f t="shared" si="58"/>
         <v>7</v>
       </c>
-      <c r="I114">
-        <f t="shared" si="47"/>
+      <c r="I142">
+        <f t="shared" si="59"/>
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
         <v>0</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B143" s="1">
         <v>1</v>
       </c>
-      <c r="C115">
-        <f t="shared" si="42"/>
+      <c r="C143">
+        <f t="shared" si="54"/>
         <v>321010</v>
       </c>
-      <c r="D115">
-        <f t="shared" si="43"/>
+      <c r="D143">
+        <f t="shared" si="55"/>
         <v>37</v>
       </c>
-      <c r="F115">
-        <f t="shared" si="44"/>
+      <c r="F143">
+        <f t="shared" si="56"/>
         <v>79</v>
       </c>
-      <c r="G115" s="1">
-        <f t="shared" si="45"/>
+      <c r="G143" s="1">
+        <f t="shared" si="57"/>
         <v>19</v>
       </c>
-      <c r="H115" s="1">
-        <f t="shared" si="46"/>
+      <c r="H143" s="1">
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
-      <c r="I115">
-        <f t="shared" si="47"/>
+      <c r="I143">
+        <f t="shared" si="59"/>
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B116" s="1">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B144" s="1">
         <v>0</v>
       </c>
-      <c r="C116">
-        <f t="shared" ref="C116" si="48">(C115+B116)*$B$3</f>
+      <c r="C144">
+        <f t="shared" ref="C144" si="60">(C143+B144)*$B$3</f>
         <v>3210100</v>
       </c>
-      <c r="D116">
-        <f t="shared" ref="D116" si="49">MOD((D115+B116)*$B$3,$B$2)</f>
+      <c r="D144">
+        <f t="shared" ref="D144" si="61">MOD((D143+B144)*$B$3,$B$2)</f>
         <v>79</v>
       </c>
-      <c r="F116">
-        <f t="shared" ref="F116" si="50">MOD(D116*$B$3,$B$2)</f>
+      <c r="F144">
+        <f t="shared" ref="F144" si="62">MOD(D144*$B$3,$B$2)</f>
         <v>14</v>
       </c>
-      <c r="G116" s="1">
-        <f t="shared" si="45"/>
+      <c r="G144" s="1">
+        <f t="shared" si="57"/>
         <v>84</v>
       </c>
-      <c r="H116" s="1">
-        <f t="shared" si="46"/>
+      <c r="H144" s="1">
+        <f t="shared" si="58"/>
         <v>8</v>
       </c>
-      <c r="I116">
-        <f t="shared" ref="I116" si="51">MOD(G116,$B$3)</f>
+      <c r="I144">
+        <f t="shared" ref="I144" si="63">MOD(G144,$B$3)</f>
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C13:C18 C94:C103">
-    <cfRule type="cellIs" dxfId="26" priority="11" operator="greaterThan">
+  <conditionalFormatting sqref="C13:C18 C94:C132">
+    <cfRule type="cellIs" dxfId="24" priority="11" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C41">
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C88">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C111:C116">
+  <conditionalFormatting sqref="C139:C144">
     <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
       <formula>$B$5</formula>
     </cfRule>

</xml_diff>

<commit_message>
Benchmarks/readme updates and new story
</commit_message>
<xml_diff>
--- a/Documentation/ISO7064ExamplesWorkbook.xlsx
+++ b/Documentation/ISO7064ExamplesWorkbook.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CheckDigits.Net\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A20487-4AB1-4E78-9B6B-86BB45230EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BC942D-44FB-49CE-BEC8-F02F13203B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{29668144-CB59-4756-8844-303BE2B9F3CC}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{29668144-CB59-4756-8844-303BE2B9F3CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="MOD 1271-36" sheetId="2" r:id="rId2"/>
-    <sheet name="MOD 661-26" sheetId="3" r:id="rId3"/>
-    <sheet name="MOD 97-10" sheetId="4" r:id="rId4"/>
-    <sheet name="MOD 11,10" sheetId="5" r:id="rId5"/>
-    <sheet name="MOD 27,26" sheetId="6" r:id="rId6"/>
-    <sheet name="MOD 37,36" sheetId="7" r:id="rId7"/>
-    <sheet name="Danish MOD 29-2" sheetId="8" r:id="rId8"/>
+    <sheet name="MOD 37-2" sheetId="9" r:id="rId2"/>
+    <sheet name="MOD 1271-36" sheetId="2" r:id="rId3"/>
+    <sheet name="MOD 661-26" sheetId="3" r:id="rId4"/>
+    <sheet name="MOD 97-10" sheetId="4" r:id="rId5"/>
+    <sheet name="MOD 11,10" sheetId="5" r:id="rId6"/>
+    <sheet name="MOD 27,26" sheetId="6" r:id="rId7"/>
+    <sheet name="MOD 37,36" sheetId="7" r:id="rId8"/>
+    <sheet name="Danish MOD 29-2" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="96">
   <si>
     <t>A</t>
   </si>
@@ -316,6 +317,21 @@
   </si>
   <si>
     <t>Additional values for Alphanumeric Mod 97-10</t>
+  </si>
+  <si>
+    <t>ISO/IEC 7064 MOD 37-2</t>
+  </si>
+  <si>
+    <t>A999914123456</t>
+  </si>
+  <si>
+    <t>Start Offsets</t>
+  </si>
+  <si>
+    <t>Check Char</t>
+  </si>
+  <si>
+    <t>A999922654321</t>
   </si>
 </sst>
 </file>
@@ -1168,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89D0F3D-CC63-4CE8-A289-1E368BD8F169}">
   <dimension ref="A2:Y120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7094,11 +7110,1278 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97FC641-D9E8-408E-8FF8-7076176893F9}">
+  <dimension ref="A1:N66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:F66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1">
+        <f>TRUNC(2147483647/B3)</f>
+        <v>1073741823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <f>MID($B$9,$N13,1)</f>
+        <v>A</v>
+      </c>
+      <c r="B14" s="1">
+        <f>LOOKUP(A14,J$13:J$49,K$13:K$49)</f>
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <f>(C13+B14)*$B$3</f>
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <f>MOD((D13+B14)*$B$3,$B$2)</f>
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <f>MOD(($B$2-D14+1),$B$2)</f>
+        <v>18</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f>LOOKUP(E14,K$13:K$49,J$13:J$49)</f>
+        <v>I</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f t="shared" ref="A15:B29" si="0">MID($B$9,$N14,1)</f>
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:C26" si="1">(C14+B15)*$B$3</f>
+        <v>58</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:D26" si="2">MOD((D14+B15)*$B$3,$B$2)</f>
+        <v>21</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:E26" si="3">MOD(($B$2-D15+1),$B$2)</f>
+        <v>17</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <f t="shared" ref="F15:F26" si="4">LOOKUP(E15,K$13:K$49,J$13:J$49)</f>
+        <v>H</v>
+      </c>
+      <c r="J15" s="1">
+        <v>2</v>
+      </c>
+      <c r="K15" s="1">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>134</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>F</v>
+      </c>
+      <c r="J16" s="1">
+        <v>3</v>
+      </c>
+      <c r="K16" s="1">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>286</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>B</v>
+      </c>
+      <c r="J17" s="1">
+        <v>4</v>
+      </c>
+      <c r="K17" s="1">
+        <v>4</v>
+      </c>
+      <c r="N17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>590</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="J18" s="1">
+        <v>5</v>
+      </c>
+      <c r="K18" s="1">
+        <v>5</v>
+      </c>
+      <c r="N18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>1182</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="J19" s="1">
+        <v>6</v>
+      </c>
+      <c r="K19" s="1">
+        <v>6</v>
+      </c>
+      <c r="N19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>2372</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>Y</v>
+      </c>
+      <c r="J20" s="1">
+        <v>7</v>
+      </c>
+      <c r="K20" s="1">
+        <v>7</v>
+      </c>
+      <c r="N20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>4746</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>S</v>
+      </c>
+      <c r="J21" s="1">
+        <v>8</v>
+      </c>
+      <c r="K21" s="1">
+        <v>8</v>
+      </c>
+      <c r="N21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>9496</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>E</v>
+      </c>
+      <c r="J22" s="1">
+        <v>9</v>
+      </c>
+      <c r="K22" s="1">
+        <v>9</v>
+      </c>
+      <c r="N22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>18998</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>L</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>10</v>
+      </c>
+      <c r="N23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="str">
+        <f>MID($B$9,$N23,1)</f>
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f>MID($B$9,$N23,1)</f>
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>38004</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>X</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1">
+        <v>11</v>
+      </c>
+      <c r="N24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>76018</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="F25" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>I</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K25" s="1">
+        <v>12</v>
+      </c>
+      <c r="N25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>152048</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="F26" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>N</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26" s="1">
+        <v>13</v>
+      </c>
+      <c r="N26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="1">
+        <v>14</v>
+      </c>
+      <c r="N27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K28" s="1">
+        <v>15</v>
+      </c>
+      <c r="N28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="1">
+        <v>16</v>
+      </c>
+      <c r="N29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" s="1">
+        <v>17</v>
+      </c>
+      <c r="N30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31" s="1">
+        <v>18</v>
+      </c>
+      <c r="N31">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" s="1">
+        <v>19</v>
+      </c>
+      <c r="N32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" t="s">
+        <v>94</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K33" s="1">
+        <v>20</v>
+      </c>
+      <c r="N33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="str">
+        <f>MID($B$29,$N13,1)</f>
+        <v>A</v>
+      </c>
+      <c r="B34" s="1">
+        <f>LOOKUP(A34,J$13:J$49,K$13:K$49)</f>
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <f>(C33+B34)*$B$3</f>
+        <v>20</v>
+      </c>
+      <c r="D34">
+        <f>MOD((D33+B34)*$B$3,$B$2)</f>
+        <v>20</v>
+      </c>
+      <c r="E34">
+        <f>MOD(($B$2-D34+1),$B$2)</f>
+        <v>18</v>
+      </c>
+      <c r="F34" s="1" t="str">
+        <f>LOOKUP(E34,K$13:K$49,J$13:J$49)</f>
+        <v>I</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="1">
+        <v>21</v>
+      </c>
+      <c r="N34">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="str">
+        <f t="shared" ref="A35:B46" si="5">MID($B$29,$N14,1)</f>
+        <v>9</v>
+      </c>
+      <c r="B35" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:C46" si="6">(C34+B35)*$B$3</f>
+        <v>58</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35:D46" si="7">MOD((D34+B35)*$B$3,$B$2)</f>
+        <v>21</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ref="E35:E46" si="8">MOD(($B$2-D35+1),$B$2)</f>
+        <v>17</v>
+      </c>
+      <c r="F35" s="1" t="str">
+        <f t="shared" ref="F35:F46" si="9">LOOKUP(E35,K$13:K$49,J$13:J$49)</f>
+        <v>H</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="1">
+        <v>22</v>
+      </c>
+      <c r="N35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="6"/>
+        <v>134</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="7"/>
+        <v>23</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="F36" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>F</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="1">
+        <v>23</v>
+      </c>
+      <c r="N36">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B37" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="6"/>
+        <v>286</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="7"/>
+        <v>27</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="F37" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>B</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K37" s="1">
+        <v>24</v>
+      </c>
+      <c r="N37">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B38" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="6"/>
+        <v>590</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="7"/>
+        <v>35</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="F38" s="1">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38" s="1">
+        <v>25</v>
+      </c>
+      <c r="N38">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="B39" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="6"/>
+        <v>1184</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="1">
+        <v>26</v>
+      </c>
+      <c r="N39">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="6"/>
+        <v>2372</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="8"/>
+        <v>34</v>
+      </c>
+      <c r="F40" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Y</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K40" s="1">
+        <v>27</v>
+      </c>
+      <c r="N40">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B41" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="6"/>
+        <v>4756</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="F41" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>I</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K41" s="1">
+        <v>28</v>
+      </c>
+      <c r="N41">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B42" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="6"/>
+        <v>9522</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="F42" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>P</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" s="1">
+        <v>29</v>
+      </c>
+      <c r="N42">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="B43" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="6"/>
+        <v>19052</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="7"/>
+        <v>34</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="F43" s="1">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K43" s="1">
+        <v>30</v>
+      </c>
+      <c r="N43">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B44" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="6"/>
+        <v>38110</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F44" s="1">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K44" s="1">
+        <v>31</v>
+      </c>
+      <c r="N44">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="B45" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="6"/>
+        <v>76224</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="8"/>
+        <v>34</v>
+      </c>
+      <c r="F45" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>Y</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K45" s="1">
+        <v>32</v>
+      </c>
+      <c r="N45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="B46" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="6"/>
+        <v>152450</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="8"/>
+        <v>28</v>
+      </c>
+      <c r="F46" s="1" t="str">
+        <f t="shared" si="9"/>
+        <v>S</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K46" s="1">
+        <v>33</v>
+      </c>
+      <c r="N46">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K47" s="1">
+        <v>34</v>
+      </c>
+      <c r="N47">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K48" s="1">
+        <v>35</v>
+      </c>
+      <c r="N48">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="J49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K49" s="1">
+        <v>36</v>
+      </c>
+      <c r="N49">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="F66" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D67299-40B5-46D7-8C2D-E7BD98472505}">
   <dimension ref="A1:P187"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14035,7 +15318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A402F48E-7D2E-4A97-B8F3-3C3001D1588A}">
   <dimension ref="A1:O165"/>
   <sheetViews>
@@ -19595,11 +20878,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF67E24C-1E84-413B-9210-17598F74D757}">
   <dimension ref="A1:M144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+    <sheetView topLeftCell="A93" workbookViewId="0">
       <selection activeCell="I107" sqref="I107:I132"/>
     </sheetView>
   </sheetViews>
@@ -23477,7 +24760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5584CF-414C-4EBC-8048-68A52149ECD3}">
   <dimension ref="A1:H122"/>
   <sheetViews>
@@ -25894,7 +27177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947D9567-54F5-4216-AEA8-9692E2EF65CA}">
   <dimension ref="A1:M167"/>
   <sheetViews>
@@ -30388,7 +31671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D6287D-4D2F-4608-A67B-E4FAB43D7DD5}">
   <dimension ref="A1:N186"/>
   <sheetViews>
@@ -35531,7 +36814,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F5BABD-809B-47ED-BCA9-0B303830648B}">
   <dimension ref="A1:O40"/>
   <sheetViews>

</xml_diff>